<commit_message>
e-Questrain/components/navbar: Items now have point cusor on hover and menu items now bolded on hover
</commit_message>
<xml_diff>
--- a/e-Question - To do list.xlsx
+++ b/e-Question - To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6219720-A590-6A4B-913A-4F65A62126CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB0BD68-C3A2-1E4A-928D-93475191A4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="198">
   <si>
     <t>Sections</t>
   </si>
@@ -680,7 +680,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -740,7 +740,7 @@
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -748,21 +748,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2251,7 +2239,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43044C79-2A71-D243-8488-97BD0DAABF7D}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43044C79-2A71-D243-8488-97BD0DAABF7D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -2290,10 +2278,10 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Priority score" fld="8" baseField="0" baseItem="0" numFmtId="165"/>
+    <dataField name="Sum of Priority score" fld="8" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -3075,8 +3063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3255,34 +3243,37 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>45</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="5">
         <f>VLOOKUP(F6,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G6,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H6,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>72</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4344,7 +4335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>44</v>
       </c>
@@ -4455,7 +4446,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>49</v>
       </c>
@@ -4482,7 +4473,7 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>74</v>
       </c>
@@ -4566,7 +4557,7 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>81</v>
       </c>
@@ -4593,7 +4584,7 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>87</v>
       </c>
@@ -4737,7 +4728,7 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>20</v>
       </c>
@@ -4797,7 +4788,7 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>66</v>
       </c>
@@ -5061,7 +5052,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>97</v>
       </c>
@@ -5181,7 +5172,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>103</v>
       </c>
@@ -5211,7 +5202,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>104</v>
       </c>
@@ -5268,7 +5259,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>38</v>
       </c>
@@ -5439,7 +5430,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>37</v>
       </c>
@@ -5499,7 +5490,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>50</v>
       </c>
@@ -5529,7 +5520,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>56</v>
       </c>
@@ -5556,7 +5547,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>41</v>
       </c>
@@ -5586,7 +5577,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>52</v>
       </c>
@@ -5613,7 +5604,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>65</v>
       </c>
@@ -5640,7 +5631,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>83</v>
       </c>
@@ -5694,7 +5685,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>105</v>
       </c>
@@ -5721,7 +5712,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>33</v>
       </c>
@@ -5748,7 +5739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>62</v>
       </c>
@@ -5772,7 +5763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>63</v>
       </c>
@@ -5796,7 +5787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>82</v>
       </c>
@@ -5823,7 +5814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>99</v>
       </c>
@@ -5985,7 +5976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>69</v>
       </c>
@@ -6039,7 +6030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
sigmafox/modals/signin: Fix issue where registration status was not reverting and the form was submitting twice on attemption to regsiter (second was a pure sign in attempt)
</commit_message>
<xml_diff>
--- a/e-Question - To do list.xlsx
+++ b/e-Question - To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB0BD68-C3A2-1E4A-928D-93475191A4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7ACAD5-1B6B-3A4C-BCD8-318C8451A605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="198">
   <si>
     <t>Sections</t>
   </si>
@@ -748,7 +748,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -766,7 +772,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45295.726403009263" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="109" xr:uid="{7B117946-7A01-F448-A249-BC4F468B572A}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45299.411269328702" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="109" xr:uid="{7B117946-7A01-F448-A249-BC4F468B572A}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:K1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
@@ -819,6 +825,162 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="109">
   <r>
+    <n v="53"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <s v="Cancelling/Voiding"/>
+    <s v="If an appointment is cancelled but that have been cancelled - then this needs to be credit noted"/>
+    <s v="Does not function as expected"/>
+    <s v="USP"/>
+    <s v="Major change to current component"/>
+    <n v="200"/>
+    <n v="77"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="Navbar"/>
+    <s v="Login Button"/>
+    <m/>
+    <s v="Should be added to Navbar"/>
+    <s v="Poor UX"/>
+    <s v="New feature"/>
+    <s v="Minor change to current component"/>
+    <n v="98"/>
+    <n v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="77"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="Voiding payments does not work"/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Investigation and change"/>
+    <n v="96"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="90"/>
+    <s v="Clients"/>
+    <s v="Client modal"/>
+    <m/>
+    <s v="Remove client is not working"/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Investigation and change"/>
+    <n v="96"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <s v="Date picker"/>
+    <s v="Should have a date picker at the top of the calendar"/>
+    <s v="Poor UX"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Minor change to current component"/>
+    <n v="72"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <s v="Navbar"/>
+    <s v="Logo "/>
+    <m/>
+    <s v="On hovering the logo the cursor should be pointer"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor tweak"/>
+    <n v="64"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <m/>
+    <s v="After trying to register (and assuming it fails) and attempts in future to sign in will result in a registration attempt"/>
+    <s v="Breaks App"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="53.333333333333336"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="59"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="The detail should reference the instructor"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Minor change to current component"/>
+    <n v="50"/>
+    <n v="60"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="60"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="New appointments should be able select an instructor"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Minor change to current component"/>
+    <n v="50"/>
+    <n v="62"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="New appointments should be able select an horse"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Minor change to current component"/>
+    <n v="50"/>
+    <n v="63"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="64"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="The detail should reference the horse"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Minor change to current component"/>
+    <n v="50"/>
+    <n v="61"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="Not able to scroll down the calendar when required"/>
+    <s v="Does not function as expected"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="42.666666666666664"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
     <n v="1"/>
     <s v="Marketing"/>
     <s v="Landing Page"/>
@@ -884,16 +1046,29 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="6"/>
-    <s v="Navbar"/>
-    <s v="Login Button"/>
-    <m/>
-    <s v="Should be added to Navbar"/>
+    <n v="24"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="User details modal"/>
+    <s v="After registering - User should be presented with a basis users detail form with:_x000a_First name_x000a_Last name_x000a_Contact number_x000a_User should also presented the option to skip_x000a_Should be place on top of the main menu page (for now - will be replaced by dash board)"/>
     <s v="Poor UX"/>
     <s v="New feature"/>
+    <s v="New component/service with simple integration"/>
+    <n v="39.200000000000003"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <s v="Navbar"/>
+    <s v="Drop down menu"/>
+    <s v="Log out"/>
+    <s v="Menu should have a log out option"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
     <s v="Minor change to current component"/>
-    <n v="98"/>
-    <n v="1"/>
+    <n v="32"/>
+    <m/>
     <x v="0"/>
   </r>
   <r>
@@ -906,19 +1081,6 @@
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
     <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="8"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="Login error warnings"/>
-    <s v="Error modals"/>
-    <s v="Poor UX"/>
-    <s v="New feature"/>
-    <s v="New component/service with complex integration"/>
-    <n v="28"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1027,6 +1189,318 @@
     <x v="0"/>
   </r>
   <r>
+    <n v="23"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="Register"/>
+    <s v="Clicking Register should warn user before it does"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <s v="Navbar"/>
+    <s v="Drop down menu"/>
+    <m/>
+    <s v="The menu hamburger should not be available if on the main menu (make no sense)"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="54"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="Invoices appointments should display the invoice number when the details are views - not to be edited"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="55"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="Invoiced appointments should be marked in some way (consider an asterisk)"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="Should show a_x000a_Pre-tax sub-total_x000a_Tax (vat) line_x000a_A grand total line"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="67"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="Should have an option to go back to the invoice list"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="84"/>
+    <s v="Clients"/>
+    <s v="Client lists"/>
+    <m/>
+    <s v="When clicking the client - it should open the modal as it does now, but in view only mode"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="89"/>
+    <s v="Clients"/>
+    <s v="Client lists"/>
+    <m/>
+    <s v="Should have an option to add a new client on this list"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="107"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment list"/>
+    <m/>
+    <s v="Should be able to toggel view to see voided payments or not (default without)"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="108"/>
+    <s v="Clients"/>
+    <s v="Client lists"/>
+    <m/>
+    <s v="Should be able to toggel view to see voided &quot;archived&quot; clients or not (default without)"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="32"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="Login error warnings"/>
+    <s v="Error modals"/>
+    <s v="Poor UX"/>
+    <s v="New feature"/>
+    <s v="New component/service with complex integration"/>
+    <n v="28"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <m/>
+    <s v="On small devices the inputs on the modal are mis-aligned (Use 340*635 spec)"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="27"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="The heights of the appointment blocks should match there duration"/>
+    <s v="Poor UI"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="27"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="When too many appointment in a slot - the blocks become cramped… need to find a more elegant way to stack appointment blocks when there are too many appointments"/>
+    <s v="Poor UI"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="27"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="The cancel changes button on and edited appointment should be darker"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="27"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="57"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="Lesson (and other sub headings) should be underlined"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="27"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="106"/>
+    <s v="General"/>
+    <m/>
+    <m/>
+    <s v="Update favicon with new logo"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="27"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="When changes are made - the save button appears - but it should always appear - just be disabled"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="74"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices parms"/>
+    <s v="On smaller screens you can see the whole modal and scroll down"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="79"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="On viewing a payment - When trying to record a new payment - the details of the old payment are brought up (as well at the void button)"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="80"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="On the statement when you click an invoice - you view the invoice detail - but when you click back it doesn't take you to the statement"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="81"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="On the statement when you click an payment - you view the payment modal - but when you click back it doesn't take you to the statement"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="87"/>
+    <s v="Clients"/>
+    <s v="Client modal"/>
+    <m/>
+    <s v="On viewing a client - When trying to record a new client - the details of the old cleint are brought up"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="88"/>
+    <s v="Clients"/>
+    <s v="Client modal"/>
+    <m/>
+    <s v="On cancelling adding a new client, should take you menu not the list (if you can from the menu)"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
     <n v="17"/>
     <s v="User Management"/>
     <s v="Sign in Modal"/>
@@ -1092,172 +1566,198 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="22"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <m/>
-    <s v="On small devices the inputs on the modal are mis-aligned (Use 340*635 spec)"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="27"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="23"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="Register"/>
-    <s v="Clicking Register should warn user before it does"/>
+    <n v="66"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="On clicking the lesson on the the viewed invoice - Should bring up the appointment modal - with no option to edit"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Minor change to current component"/>
+    <n v="18"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="76"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment view"/>
+    <m/>
+    <s v="On clicking the payment on the payment list - Should the payment modal in view only mode"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Minor change to current component"/>
+    <n v="18"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="73"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices parms"/>
+    <s v="The generate invoices button should not be available if the form is not completed correctly"/>
     <s v="Poor UX"/>
     <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="24"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="User details modal"/>
-    <s v="After registering - User should be presented with a basis users detail form with:_x000a_First name_x000a_Last name_x000a_Contact number_x000a_User should also presented the option to skip_x000a_Should be place on top of the main menu page (for now - will be replaced by dash board)"/>
-    <s v="Poor UX"/>
-    <s v="New feature"/>
-    <s v="New component/service with simple integration"/>
-    <n v="39.200000000000003"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="25"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <m/>
-    <s v="After trying to register (and assuming it fails) and attempts in future to sign in will result in a registration attempt"/>
-    <s v="Breaks App"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="53.333333333333336"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="26"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Main menu"/>
-    <m/>
-    <s v="As the screen gets wider - the buttons tend to lower - needs to be consistent"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Investigation and change"/>
-    <n v="9"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="27"/>
-    <s v="General"/>
-    <s v="Utility services"/>
-    <m/>
-    <s v="There needs to be a service that determine whether the view should be mobile or desktop"/>
-    <s v="Poor UI"/>
-    <s v="Refactor/Tech debt"/>
-    <s v="New component/service with complex integration"/>
-    <n v="0.42857142857142855"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="28"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Main menu"/>
-    <m/>
-    <s v="There should be a view for desktop where the button become a grid of square buttons with icons"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
     <s v="Major change to current component"/>
-    <n v="6.75"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="29"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Main menu"/>
-    <m/>
-    <s v="Needs to use the new view service to determine its required state"/>
-    <s v="Poor UI"/>
-    <s v="Refactor/Tech debt"/>
-    <s v="Minor change to current component"/>
-    <n v="1.5"/>
-    <n v="27"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="30"/>
-    <s v="Navbar"/>
-    <m/>
-    <m/>
-    <s v="Needs to use the new view service to determine its required state"/>
-    <s v="Poor UI"/>
-    <s v="Refactor/Tech debt"/>
-    <s v="Minor change to current component"/>
-    <n v="1.5"/>
-    <n v="27"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="31"/>
-    <s v="Navbar"/>
-    <s v="Drop down menu"/>
-    <m/>
-    <s v="The menu hamburger should not be available if on the main menu (make no sense)"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="32"/>
-    <s v="Navbar"/>
-    <s v="Logo "/>
-    <m/>
-    <s v="On hovering the logo the cursor should be pointer"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor tweak"/>
-    <n v="64"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="33"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Dashboard"/>
-    <m/>
-    <s v="New page: Dashboard_x000a_Should only be available on desktop_x000a_Should have a option to go to the main menu_x000a_Will contain a variety of reports and summaries"/>
+    <n v="16"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="91"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Review by instructor"/>
+    <m/>
+    <s v="Required to be built"/>
     <s v="Nice to have"/>
     <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="10"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="34"/>
-    <s v="Navbar"/>
-    <s v="Drop down menu"/>
-    <s v="Log out"/>
-    <s v="Menu should have a log out option"/>
-    <s v="Poor UX"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Minor change to current component"/>
-    <n v="72"/>
-    <m/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="59"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="92"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Review by horse"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="64"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="93"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Expenses by instructor"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="59"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Expenses by horse"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="64"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="95"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Contribution by instructor"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="59"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="96"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Contribution by horse"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="64"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="97"/>
+    <s v="Finance - Accounting"/>
+    <s v="Bank statement importer"/>
+    <m/>
+    <s v="If expenses are allocated to instrutors should be able to allocate per instructor"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="59"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <s v="Finance - Accounting"/>
+    <s v="Bank statement importer"/>
+    <m/>
+    <s v="If expenses are allocated to instrutors should be able to allocate per instructor"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="64"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="100"/>
+    <s v="Clients"/>
+    <s v="Lesson booking platform"/>
+    <m/>
+    <s v="On adding a new client - the client needs to be sent and email/sms/text with a link to where they can book their own lessons"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="99"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="101"/>
+    <s v="Clients"/>
+    <s v="Lesson booking platform"/>
+    <m/>
+    <s v="Client should be able to add themselves as a new client - when on on the booking platform"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="100"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="103"/>
+    <s v="Finance - Accounting"/>
+    <s v="Statement runs"/>
+    <m/>
+    <s v="Should be able perform a link batch dispurse where the use is sent a link to where their invoices can be found on the platform"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="102"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="104"/>
+    <s v="Finance - Accounting"/>
+    <s v="Statement runs"/>
+    <m/>
+    <s v="Should be able to email the documents and statements to the client"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="14.285714285714286"/>
+    <n v="103"/>
     <x v="0"/>
   </r>
   <r>
@@ -1266,6 +1766,71 @@
     <s v="Drop down menu"/>
     <m/>
     <s v="Should not down the screen - but should hover above the current screen content"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="On taller screens - the schedule slots should be have a great height to fill the remainder of the screen"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="71"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices parms"/>
+    <s v="The radio should be better group - they are too far apart to make sense"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="72"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices parms"/>
+    <s v="Group of buttons should have a little border to show better raltions logic"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="85"/>
+    <s v="Clients"/>
+    <s v="Client lists"/>
+    <m/>
+    <s v="List on smaller screens are squashed"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="86"/>
+    <s v="Clients"/>
+    <s v="Client lists"/>
+    <m/>
+    <s v="Lines on the list should have alternating colours"/>
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor change to current component"/>
@@ -1300,41 +1865,41 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="38"/>
+    <n v="47"/>
     <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="On taller screens - the schedule slots should be have a great height to fill the remainder of the screen"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="39"/>
+    <s v="Appointments modal"/>
+    <s v="Cancelling/Voiding"/>
+    <s v="Cancelling the appointment should warn the user before the appointment is actually cancelled"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="New component/service with simple integration"/>
+    <n v="12.8"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="50"/>
     <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="On shorter screens - Schedule slot should have a minimum height"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Investigation and change"/>
-    <n v="9"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="40"/>
+    <s v="Appointments modal"/>
+    <s v="Cancelling/Voiding"/>
+    <s v="On cancelling a new appointment (after changes are made) should warn the user that changes will be lost"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="New component/service with simple integration"/>
+    <n v="12.8"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="56"/>
     <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="Not able to scroll down the calendar when required"/>
-    <s v="Does not function as expected"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="When cancelling an invoiced appoint and additional warning of the credit not needs to be provided"/>
+    <s v="Poor UX"/>
     <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="42.666666666666664"/>
+    <s v="New component/service with simple integration"/>
+    <n v="12.8"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1352,6 +1917,162 @@
     <x v="0"/>
   </r>
   <r>
+    <n v="52"/>
+    <s v="Finance - Payments"/>
+    <s v="Bulk uploads"/>
+    <m/>
+    <s v="Should be able to bulk upload payments_x000a_Should have a standard template_x000a_Should remember the reference - and assign based on that (where this has been seen before)"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="65"/>
+    <s v="Finance - Invoicing"/>
+    <s v="PDF export"/>
+    <m/>
+    <s v="Should be able to export the invoice to PDF_x000a_Will required a lot more client and company detail_x000a_Should ask the user where to save it"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="83"/>
+    <s v="Finance - Reports"/>
+    <s v="Profit and lose report"/>
+    <m/>
+    <s v="Mini profit and loss report_x000a_Should be able to select for a period "/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="102"/>
+    <s v="Finance - Accounting"/>
+    <s v="Statement runs"/>
+    <m/>
+    <s v="Client should be able to perform a statement run with a simple flow process_x000a_All clients statements are to be PDDd and saved to their folder along with their backing fin documents (invoice, credit notes etc , payment receipts)_x000a_User should be able to determine where the batch of documents is saved"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="105"/>
+    <s v="User Management"/>
+    <s v="Profile portal"/>
+    <m/>
+    <s v="A portal where the client can_x000a_Update their details_x000a_Add new users to their account_x000a_Any other preferances they want"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Dashboard"/>
+    <m/>
+    <s v="New page: Dashboard_x000a_Should only be available on desktop_x000a_Should have a option to go to the main menu_x000a_Will contain a variety of reports and summaries"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="10"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="62"/>
+    <s v="Equipment/Assets"/>
+    <m/>
+    <m/>
+    <s v="New section required to add instructor to the client"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="10"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="63"/>
+    <s v="Staff management"/>
+    <m/>
+    <m/>
+    <s v="New section required to add horse to the client"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="10"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="82"/>
+    <s v="Finance - Accounting"/>
+    <s v="Bank statement importer"/>
+    <m/>
+    <s v="Should be able import a bank statement:_x000a_Would require use to allocate transactions_x000a_Transaction are to be remembered for future use_x000a_Should perform a quick recon calculation_x000a_Expenses should be able to be caputured when paid (Later wil be done on a inoice basis and then payments are allocated to supplier dues)"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="10"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="99"/>
+    <s v="Booking"/>
+    <s v="Lesson booking platform"/>
+    <m/>
+    <s v="A platform where a customer of the client can book their lessions, based on the slots the client has deemed and allowed as open"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="10"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Main menu"/>
+    <m/>
+    <s v="As the screen gets wider - the buttons tend to lower - needs to be consistent"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Investigation and change"/>
+    <n v="9"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="On shorter screens - Schedule slot should have a minimum height"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Investigation and change"/>
+    <n v="9"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
     <n v="42"/>
     <s v="Calendar/Appointments"/>
     <s v="Appointments modal"/>
@@ -1365,45 +2086,6 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="43"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="The heights of the appointment blocks should match there duration"/>
-    <s v="Poor UI"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="27"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="44"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="When too many appointment in a slot - the blocks become cramped… need to find a more elegant way to stack appointment blocks when there are too many appointments"/>
-    <s v="Poor UI"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="27"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="45"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <s v="Date picker"/>
-    <s v="Should have a date picker at the top of the calendar"/>
-    <s v="Poor UX"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Minor change to current component"/>
-    <n v="72"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
     <n v="46"/>
     <s v="Calendar/Appointments"/>
     <s v="Appointments modal"/>
@@ -1417,279 +2099,6 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="47"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <s v="Cancelling/Voiding"/>
-    <s v="Cancelling the appointment should warn the user before the appointment is actually cancelled"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="New component/service with simple integration"/>
-    <n v="12.8"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="48"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="The cancel changes button on and edited appointment should be darker"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="27"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="49"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="When changes are made - the save button appears - but it should always appear - just be disabled"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="50"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <s v="Cancelling/Voiding"/>
-    <s v="On cancelling a new appointment (after changes are made) should warn the user that changes will be lost"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="New component/service with simple integration"/>
-    <n v="12.8"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="51"/>
-    <s v="General"/>
-    <s v="Warnings"/>
-    <m/>
-    <s v="Warnings should have an option to allow users to not see them again"/>
-    <s v="Nice to have"/>
-    <s v="New feature"/>
-    <s v="New component/service with complex integration"/>
-    <n v="7"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="52"/>
-    <s v="Finance - Payments"/>
-    <s v="Bulk uploads"/>
-    <m/>
-    <s v="Should be able to bulk upload payments_x000a_Should have a standard template_x000a_Should remember the reference - and assign based on that (where this has been seen before)"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="53"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <s v="Cancelling/Voiding"/>
-    <s v="If an appointment is cancelled but that have been cancelled - then this needs to be credit noted"/>
-    <s v="Does not function as expected"/>
-    <s v="USP"/>
-    <s v="Major change to current component"/>
-    <n v="200"/>
-    <n v="77"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="54"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="Invoices appointments should display the invoice number when the details are views - not to be edited"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="55"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="Invoiced appointments should be marked in some way (consider an asterisk)"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="56"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="When cancelling an invoiced appoint and additional warning of the credit not needs to be provided"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="New component/service with simple integration"/>
-    <n v="12.8"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="57"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="Lesson (and other sub headings) should be underlined"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="27"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="58"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="Should show a_x000a_Pre-tax sub-total_x000a_Tax (vat) line_x000a_A grand total line"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="59"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="The detail should reference the instructor"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Minor change to current component"/>
-    <n v="50"/>
-    <n v="60"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="60"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="New appointments should be able select an instructor"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Minor change to current component"/>
-    <n v="50"/>
-    <n v="62"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="61"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="New appointments should be able select an horse"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Minor change to current component"/>
-    <n v="50"/>
-    <n v="63"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="62"/>
-    <s v="Equipment/Assets"/>
-    <m/>
-    <m/>
-    <s v="New section required to add instructor to the client"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="10"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="63"/>
-    <s v="Staff management"/>
-    <m/>
-    <m/>
-    <s v="New section required to add horse to the client"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="10"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="64"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="The detail should reference the horse"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Minor change to current component"/>
-    <n v="50"/>
-    <n v="61"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="65"/>
-    <s v="Finance - Invoicing"/>
-    <s v="PDF export"/>
-    <m/>
-    <s v="Should be able to export the invoice to PDF_x000a_Will required a lot more client and company detail_x000a_Should ask the user where to save it"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="66"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="On clicking the lesson on the the viewed invoice - Should bring up the appointment modal - with no option to edit"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Minor change to current component"/>
-    <n v="18"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="67"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="Should have an option to go back to the invoice list"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
     <n v="68"/>
     <s v="Finance - Invoicing"/>
     <s v="Invoice list"/>
@@ -1725,58 +2134,6 @@
     <s v="Feature enhancement/fix"/>
     <s v="Major change to current component"/>
     <n v="9"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="71"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices parms"/>
-    <s v="The radio should be better group - they are too far apart to make sense"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="72"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices parms"/>
-    <s v="Group of buttons should have a little border to show better raltions logic"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="73"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices parms"/>
-    <s v="The generate invoices button should not be available if the form is not completed correctly"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Major change to current component"/>
-    <n v="16"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="74"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices parms"/>
-    <s v="On smaller screens you can see the whole modal and scroll down"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="21.333333333333332"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1794,32 +2151,6 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="76"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment view"/>
-    <m/>
-    <s v="On clicking the payment on the payment list - Should the payment modal in view only mode"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Minor change to current component"/>
-    <n v="18"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="77"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment modal"/>
-    <m/>
-    <s v="Voiding payments does not work"/>
-    <s v="Does not function as expected"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Investigation and change"/>
-    <n v="96"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
     <n v="78"/>
     <s v="Finance - Payments"/>
     <s v="Payment modal"/>
@@ -1833,392 +2164,67 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="79"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment modal"/>
-    <m/>
-    <s v="On viewing a payment - When trying to record a new payment - the details of the old payment are brought up (as well at the void button)"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="80"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="On the statement when you click an invoice - you view the invoice detail - but when you click back it doesn't take you to the statement"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="81"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment modal"/>
-    <m/>
-    <s v="On the statement when you click an payment - you view the payment modal - but when you click back it doesn't take you to the statement"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="82"/>
-    <s v="Finance - Accounting"/>
-    <s v="Bank statement importer"/>
-    <m/>
-    <s v="Should be able import a bank statement:_x000a_Would require use to allocate transactions_x000a_Transaction are to be remembered for future use_x000a_Should perform a quick recon calculation_x000a_Expenses should be able to be caputured when paid (Later wil be done on a inoice basis and then payments are allocated to supplier dues)"/>
+    <n v="51"/>
+    <s v="General"/>
+    <s v="Warnings"/>
+    <m/>
+    <s v="Warnings should have an option to allow users to not see them again"/>
     <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="10"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="83"/>
-    <s v="Finance - Reports"/>
-    <s v="Profit and lose report"/>
-    <m/>
-    <s v="Mini profit and loss report_x000a_Should be able to select for a period "/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="84"/>
-    <s v="Clients"/>
-    <s v="Client lists"/>
-    <m/>
-    <s v="When clicking the client - it should open the modal as it does now, but in view only mode"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="85"/>
-    <s v="Clients"/>
-    <s v="Client lists"/>
-    <m/>
-    <s v="List on smaller screens are squashed"/>
+    <s v="New feature"/>
+    <s v="New component/service with complex integration"/>
+    <n v="7"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Main menu"/>
+    <m/>
+    <s v="There should be a view for desktop where the button become a grid of square buttons with icons"/>
     <s v="Poor UI"/>
     <s v="Improved UI"/>
+    <s v="Major change to current component"/>
+    <n v="6.75"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Main menu"/>
+    <m/>
+    <s v="Needs to use the new view service to determine its required state"/>
+    <s v="Poor UI"/>
+    <s v="Refactor/Tech debt"/>
     <s v="Minor change to current component"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="86"/>
-    <s v="Clients"/>
-    <s v="Client lists"/>
-    <m/>
-    <s v="Lines on the list should have alternating colours"/>
+    <n v="1.5"/>
+    <n v="27"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <s v="Navbar"/>
+    <m/>
+    <m/>
+    <s v="Needs to use the new view service to determine its required state"/>
     <s v="Poor UI"/>
-    <s v="Improved UI"/>
+    <s v="Refactor/Tech debt"/>
     <s v="Minor change to current component"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="87"/>
-    <s v="Clients"/>
-    <s v="Client modal"/>
-    <m/>
-    <s v="On viewing a client - When trying to record a new client - the details of the old cleint are brought up"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="88"/>
-    <s v="Clients"/>
-    <s v="Client modal"/>
-    <m/>
-    <s v="On cancelling adding a new client, should take you menu not the list (if you can from the menu)"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="89"/>
-    <s v="Clients"/>
-    <s v="Client lists"/>
-    <m/>
-    <s v="Should have an option to add a new client on this list"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="90"/>
-    <s v="Clients"/>
-    <s v="Client modal"/>
-    <m/>
-    <s v="Remove client is not working"/>
-    <s v="Does not function as expected"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Investigation and change"/>
-    <n v="96"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="91"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Review by instructor"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
+    <n v="1.5"/>
+    <n v="27"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <s v="General"/>
+    <s v="Utility services"/>
+    <m/>
+    <s v="There needs to be a service that determine whether the view should be mobile or desktop"/>
+    <s v="Poor UI"/>
+    <s v="Refactor/Tech debt"/>
     <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="59"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="92"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Review by horse"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="64"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="93"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Expenses by instructor"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="59"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="94"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Expenses by horse"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="64"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="95"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Contribution by instructor"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="59"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="96"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Contribution by horse"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="64"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="97"/>
-    <s v="Finance - Accounting"/>
-    <s v="Bank statement importer"/>
-    <m/>
-    <s v="If expenses are allocated to instrutors should be able to allocate per instructor"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="59"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="98"/>
-    <s v="Finance - Accounting"/>
-    <s v="Bank statement importer"/>
-    <m/>
-    <s v="If expenses are allocated to instrutors should be able to allocate per instructor"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="64"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="99"/>
-    <s v="Booking"/>
-    <s v="Lesson booking platform"/>
-    <m/>
-    <s v="A platform where a customer of the client can book their lessions, based on the slots the client has deemed and allowed as open"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="10"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="100"/>
-    <s v="Clients"/>
-    <s v="Lesson booking platform"/>
-    <m/>
-    <s v="On adding a new client - the client needs to be sent and email/sms/text with a link to where they can book their own lessons"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="99"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="101"/>
-    <s v="Clients"/>
-    <s v="Lesson booking platform"/>
-    <m/>
-    <s v="Client should be able to add themselves as a new client - when on on the booking platform"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="100"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="102"/>
-    <s v="Finance - Accounting"/>
-    <s v="Statement runs"/>
-    <m/>
-    <s v="Client should be able to perform a statement run with a simple flow process_x000a_All clients statements are to be PDDd and saved to their folder along with their backing fin documents (invoice, credit notes etc , payment receipts)_x000a_User should be able to determine where the batch of documents is saved"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="103"/>
-    <s v="Finance - Accounting"/>
-    <s v="Statement runs"/>
-    <m/>
-    <s v="Should be able perform a link batch dispurse where the use is sent a link to where their invoices can be found on the platform"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="102"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="104"/>
-    <s v="Finance - Accounting"/>
-    <s v="Statement runs"/>
-    <m/>
-    <s v="Should be able to email the documents and statements to the client"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="14.285714285714286"/>
-    <n v="103"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="105"/>
-    <s v="User Management"/>
-    <s v="Profile portal"/>
-    <m/>
-    <s v="A portal where the client can_x000a_Update their details_x000a_Add new users to their account_x000a_Any other preferances they want"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="106"/>
-    <s v="General"/>
-    <m/>
-    <m/>
-    <s v="Update favicon with new logo"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="27"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="107"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment list"/>
-    <m/>
-    <s v="Should be able to toggel view to see voided payments or not (default without)"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="108"/>
-    <s v="Clients"/>
-    <s v="Client lists"/>
-    <m/>
-    <s v="Should be able to toggel view to see voided &quot;archived&quot; clients or not (default without)"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="32"/>
+    <n v="0.42857142857142855"/>
     <m/>
     <x v="0"/>
   </r>
@@ -2239,7 +2245,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43044C79-2A71-D243-8488-97BD0DAABF7D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43044C79-2A71-D243-8488-97BD0DAABF7D}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -2281,7 +2287,7 @@
     <dataField name="Sum of Priority score" fld="8" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2597,14 +2603,15 @@
   <dimension ref="A3:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2628,19 +2635,19 @@
         <v>197</v>
       </c>
       <c r="B5" s="7">
-        <v>219</v>
+        <v>355</v>
       </c>
       <c r="C5" s="7">
-        <v>2651.9976190476191</v>
+        <v>2475.9976190476195</v>
       </c>
       <c r="D5" s="7">
-        <v>2870.9976190476191</v>
+        <v>2830.9976190476195</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D7" s="8">
         <f>GETPIVOTDATA("Priority score",$A$3,"Status","Done")/GETPIVOTDATA("Priority score",$A$3)</f>
-        <v>7.6280105057226669E-2</v>
+        <v>0.12539749154555138</v>
       </c>
     </row>
   </sheetData>
@@ -3063,7 +3070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -3276,31 +3283,34 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="5">
         <f>VLOOKUP(F7,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G7,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H7,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>64</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
e-Questrain/pages/calendarcalendar: Page now scroll to end of calendar
</commit_message>
<xml_diff>
--- a/e-Question - To do list.xlsx
+++ b/e-Question - To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7ACAD5-1B6B-3A4C-BCD8-318C8451A605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BECAFEC-5CC4-5445-ACEF-C024DB39EAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="199">
   <si>
     <t>Sections</t>
   </si>
@@ -672,6 +672,9 @@
   </si>
   <si>
     <t>Sum of Priority score</t>
+  </si>
+  <si>
+    <t>auth/network-request-failed</t>
   </si>
 </sst>
 </file>
@@ -748,13 +751,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -2245,7 +2242,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43044C79-2A71-D243-8488-97BD0DAABF7D}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43044C79-2A71-D243-8488-97BD0DAABF7D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -2287,7 +2284,7 @@
     <dataField name="Sum of Priority score" fld="8" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -3068,10 +3065,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3320,24 +3317,29 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="5">
         <f>VLOOKUP(F8,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G8,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H8,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>53.333333333333336</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -3669,19 +3671,16 @@
     </row>
     <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="F20" t="s">
         <v>15</v>
@@ -3699,7 +3698,7 @@
     </row>
     <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -3707,8 +3706,11 @@
       <c r="C21" t="s">
         <v>43</v>
       </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
       <c r="E21" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
@@ -3723,10 +3725,13 @@
         <f>VLOOKUP(F21,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G21,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H21,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="J21">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -3738,7 +3743,7 @@
         <v>45</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
@@ -3759,7 +3764,7 @@
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -3771,7 +3776,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
@@ -3792,7 +3797,7 @@
     </row>
     <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -3804,7 +3809,7 @@
         <v>45</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
@@ -3825,7 +3830,7 @@
     </row>
     <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -3837,7 +3842,7 @@
         <v>45</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
@@ -3858,7 +3863,7 @@
     </row>
     <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -3870,7 +3875,7 @@
         <v>45</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -3891,7 +3896,7 @@
     </row>
     <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -3903,7 +3908,7 @@
         <v>45</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -3924,7 +3929,7 @@
     </row>
     <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -3936,7 +3941,7 @@
         <v>45</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
@@ -3957,7 +3962,7 @@
     </row>
     <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -3966,10 +3971,10 @@
         <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
@@ -3984,25 +3989,19 @@
         <f>VLOOKUP(F29,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G29,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H29,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="J29">
-        <v>8</v>
-      </c>
     </row>
     <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -4020,7 +4019,7 @@
     </row>
     <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>39</v>
@@ -4028,8 +4027,11 @@
       <c r="C31" t="s">
         <v>81</v>
       </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
       <c r="E31" s="2" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="F31" t="s">
         <v>15</v>
@@ -4263,7 +4265,7 @@
     </row>
     <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -4274,26 +4276,29 @@
       <c r="D40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>47</v>
+      <c r="E40" t="s">
+        <v>198</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H40" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="I40" s="1">
         <f>VLOOKUP(F40,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G40,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H40,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="J40">
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -4301,44 +4306,47 @@
       <c r="C41" t="s">
         <v>43</v>
       </c>
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
       <c r="E41" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H41" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="I41" s="1">
         <f>VLOOKUP(F41,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G41,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H41,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
         <v>43</v>
       </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>88</v>
-      </c>
       <c r="E42" s="2" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="F42" t="s">
         <v>16</v>
       </c>
       <c r="G42" t="s">
-        <v>168</v>
+        <v>29</v>
       </c>
       <c r="H42" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="I42" s="1">
         <f>VLOOKUP(F42,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G42,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H42,'Source lists'!$K$2:$L$9,2,FALSE)</f>
@@ -4347,7 +4355,7 @@
     </row>
     <row r="43" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
@@ -4356,7 +4364,7 @@
         <v>88</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F43" t="s">
         <v>16</v>
@@ -4374,25 +4382,25 @@
     </row>
     <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F44" t="s">
         <v>16</v>
       </c>
       <c r="G44" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="H44" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="I44" s="1">
         <f>VLOOKUP(F44,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G44,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H44,'Source lists'!$K$2:$L$9,2,FALSE)</f>
@@ -4401,16 +4409,16 @@
     </row>
     <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F45" t="s">
         <v>16</v>
@@ -4427,77 +4435,74 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
-        <v>106</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F46" s="3" t="s">
+      <c r="A46">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>107</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G46" t="s">
         <v>29</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" t="s">
         <v>25</v>
       </c>
-      <c r="I46" s="5">
+      <c r="I46" s="1">
         <f>VLOOKUP(F46,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G46,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H46,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3" t="s">
+    </row>
+    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>106</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" s="5">
+        <f>VLOOKUP(F47,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G47,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H47,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>49</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>92</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F47" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" t="s">
-        <v>28</v>
-      </c>
-      <c r="H47" t="s">
-        <v>24</v>
-      </c>
-      <c r="I47" s="1">
-        <f>VLOOKUP(F47,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G47,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H47,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>21.333333333333332</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>138</v>
-      </c>
-      <c r="D48" t="s">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="F48" t="s">
         <v>15</v>
@@ -4515,16 +4520,19 @@
     </row>
     <row r="49" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>138</v>
+      </c>
+      <c r="D49" t="s">
+        <v>139</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="F49" t="s">
         <v>15</v>
@@ -4542,16 +4550,16 @@
     </row>
     <row r="50" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
@@ -4569,16 +4577,16 @@
     </row>
     <row r="51" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F51" t="s">
         <v>15</v>
@@ -4596,16 +4604,16 @@
     </row>
     <row r="52" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="F52" t="s">
         <v>15</v>
@@ -4623,7 +4631,7 @@
     </row>
     <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
@@ -4632,7 +4640,7 @@
         <v>162</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -4650,37 +4658,34 @@
     </row>
     <row r="54" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
-      </c>
-      <c r="D54" t="s">
-        <v>55</v>
+        <v>162</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>56</v>
+        <v>165</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
       </c>
       <c r="G54" t="s">
-        <v>168</v>
+        <v>28</v>
       </c>
       <c r="H54" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="I54" s="1">
         <f>VLOOKUP(F54,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G54,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H54,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>20.571428571428573</v>
+        <v>21.333333333333332</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -4692,7 +4697,7 @@
         <v>55</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
@@ -4710,7 +4715,7 @@
     </row>
     <row r="56" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -4722,7 +4727,7 @@
         <v>55</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
@@ -4740,7 +4745,7 @@
     </row>
     <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -4752,7 +4757,7 @@
         <v>55</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
@@ -4770,7 +4775,7 @@
     </row>
     <row r="58" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -4782,7 +4787,7 @@
         <v>55</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -4800,43 +4805,46 @@
     </row>
     <row r="59" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>43</v>
+      </c>
+      <c r="D59" t="s">
+        <v>55</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="F59" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G59" t="s">
         <v>168</v>
       </c>
       <c r="H59" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I59" s="1">
         <f>VLOOKUP(F59,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G59,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H59,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>18</v>
+        <v>20.571428571428573</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="F60" t="s">
         <v>17</v>
@@ -4854,73 +4862,70 @@
     </row>
     <row r="61" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
-      </c>
-      <c r="D61" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F61" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G61" t="s">
-        <v>28</v>
+        <v>168</v>
       </c>
       <c r="H61" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="I61" s="1">
         <f>VLOOKUP(F61,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G61,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H61,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>138</v>
+      </c>
+      <c r="D62" t="s">
+        <v>139</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="F62" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G62" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I62" s="1">
         <f>VLOOKUP(F62,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G62,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H62,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="J62">
-        <v>59</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>176</v>
@@ -4939,18 +4944,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J63">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>176</v>
@@ -4969,18 +4974,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J64">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>176</v>
@@ -4999,18 +5004,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J65">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>176</v>
@@ -5029,18 +5034,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J66">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>176</v>
@@ -5059,21 +5064,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J67">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F68" t="s">
         <v>17</v>
@@ -5089,12 +5094,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J68">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
         <v>5</v>
@@ -5119,21 +5124,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J69">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F70" t="s">
         <v>17</v>
@@ -5149,12 +5154,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J70">
-        <v>99</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
@@ -5163,7 +5168,7 @@
         <v>179</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -5179,21 +5184,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J71">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F72" t="s">
         <v>17</v>
@@ -5209,12 +5214,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J72">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
@@ -5223,7 +5228,7 @@
         <v>183</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F73" t="s">
         <v>17</v>
@@ -5239,48 +5244,51 @@
         <v>14.285714285714286</v>
       </c>
       <c r="J73">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="F74" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G74" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H74" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I74" s="1">
         <f>VLOOKUP(F74,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G74,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H74,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>13.5</v>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="J74">
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F75" t="s">
         <v>16</v>
@@ -5298,19 +5306,16 @@
     </row>
     <row r="76" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>138</v>
-      </c>
-      <c r="D76" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F76" t="s">
         <v>16</v>
@@ -5328,7 +5333,7 @@
     </row>
     <row r="77" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B77" t="s">
         <v>2</v>
@@ -5340,7 +5345,7 @@
         <v>139</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F77" t="s">
         <v>16</v>
@@ -5358,16 +5363,19 @@
     </row>
     <row r="78" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>158</v>
+        <v>138</v>
+      </c>
+      <c r="D78" t="s">
+        <v>139</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
@@ -5385,7 +5393,7 @@
     </row>
     <row r="79" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
@@ -5394,7 +5402,7 @@
         <v>158</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F79" t="s">
         <v>16</v>
@@ -5412,43 +5420,40 @@
     </row>
     <row r="80" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>74</v>
-      </c>
-      <c r="D80" t="s">
-        <v>86</v>
+        <v>158</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="F80" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G80" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H80" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="I80" s="1">
         <f>VLOOKUP(F80,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G80,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H80,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.8</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C81" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D81" t="s">
         <v>86</v>
@@ -5472,19 +5477,19 @@
     </row>
     <row r="82" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C82" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="F82" t="s">
         <v>15</v>
@@ -5502,7 +5507,7 @@
     </row>
     <row r="83" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
@@ -5514,7 +5519,7 @@
         <v>114</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="F83" t="s">
         <v>15</v>
@@ -5532,7 +5537,7 @@
     </row>
     <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
@@ -5540,8 +5545,11 @@
       <c r="C84" t="s">
         <v>92</v>
       </c>
+      <c r="D84" t="s">
+        <v>114</v>
+      </c>
       <c r="E84" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F84" t="s">
         <v>15</v>
@@ -5559,46 +5567,46 @@
     </row>
     <row r="85" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>88</v>
-      </c>
-      <c r="D85" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="F85" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G85" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H85" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="I85" s="1">
         <f>VLOOKUP(F85,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G85,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H85,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.5</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B86" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>105</v>
+        <v>88</v>
+      </c>
+      <c r="D86" t="s">
+        <v>90</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F86" t="s">
         <v>17</v>
@@ -5616,16 +5624,16 @@
     </row>
     <row r="87" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B87" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="F87" t="s">
         <v>17</v>
@@ -5643,16 +5651,16 @@
     </row>
     <row r="88" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="F88" t="s">
         <v>17</v>
@@ -5670,16 +5678,16 @@
     </row>
     <row r="89" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="F89" t="s">
         <v>17</v>
@@ -5697,16 +5705,16 @@
     </row>
     <row r="90" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B90" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F90" t="s">
         <v>17</v>
@@ -5724,16 +5732,16 @@
     </row>
     <row r="91" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="B91" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C91" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>119</v>
+        <v>188</v>
       </c>
       <c r="F91" t="s">
         <v>17</v>
@@ -5742,22 +5750,25 @@
         <v>26</v>
       </c>
       <c r="H91" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I91" s="1">
         <f>VLOOKUP(F91,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G91,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H91,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>10</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>67</v>
+      </c>
+      <c r="C92" t="s">
+        <v>83</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F92" t="s">
         <v>17</v>
@@ -5775,13 +5786,13 @@
     </row>
     <row r="93" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B93" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F93" t="s">
         <v>17</v>
@@ -5799,16 +5810,13 @@
     </row>
     <row r="94" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="F94" t="s">
         <v>17</v>
@@ -5826,16 +5834,16 @@
     </row>
     <row r="95" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B95" t="s">
-        <v>178</v>
+        <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="F95" t="s">
         <v>17</v>
@@ -5853,43 +5861,43 @@
     </row>
     <row r="96" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A96">
+        <v>99</v>
+      </c>
+      <c r="B96" t="s">
+        <v>178</v>
+      </c>
+      <c r="C96" t="s">
+        <v>179</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F96" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" t="s">
         <v>26</v>
       </c>
-      <c r="B96" t="s">
-        <v>67</v>
-      </c>
-      <c r="C96" t="s">
-        <v>74</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F96" t="s">
-        <v>16</v>
-      </c>
-      <c r="G96" t="s">
-        <v>29</v>
-      </c>
       <c r="H96" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I96" s="1">
         <f>VLOOKUP(F96,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G96,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H96,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B97" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C97" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="F97" t="s">
         <v>16</v>
@@ -5907,16 +5915,16 @@
     </row>
     <row r="98" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="F98" t="s">
         <v>16</v>
@@ -5934,7 +5942,7 @@
     </row>
     <row r="99" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B99" t="s">
         <v>1</v>
@@ -5943,7 +5951,7 @@
         <v>92</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F99" t="s">
         <v>16</v>
@@ -5961,25 +5969,25 @@
     </row>
     <row r="100" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B100" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="F100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G100" t="s">
-        <v>168</v>
+        <v>29</v>
       </c>
       <c r="H100" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="I100" s="1">
         <f>VLOOKUP(F100,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G100,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H100,'Source lists'!$K$2:$L$9,2,FALSE)</f>
@@ -5988,7 +5996,7 @@
     </row>
     <row r="101" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B101" t="s">
         <v>2</v>
@@ -5997,7 +6005,7 @@
         <v>134</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F101" t="s">
         <v>17</v>
@@ -6015,7 +6023,7 @@
     </row>
     <row r="102" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B102" t="s">
         <v>2</v>
@@ -6024,7 +6032,7 @@
         <v>134</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F102" t="s">
         <v>17</v>
@@ -6042,19 +6050,16 @@
     </row>
     <row r="103" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B103" t="s">
         <v>2</v>
       </c>
       <c r="C103" t="s">
-        <v>138</v>
-      </c>
-      <c r="D103" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F103" t="s">
         <v>17</v>
@@ -6072,16 +6077,19 @@
     </row>
     <row r="104" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B104" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C104" t="s">
-        <v>149</v>
+        <v>138</v>
+      </c>
+      <c r="D104" t="s">
+        <v>144</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F104" t="s">
         <v>17</v>
@@ -6099,61 +6107,61 @@
     </row>
     <row r="105" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B105" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>103</v>
+        <v>149</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="F105" t="s">
         <v>17</v>
       </c>
       <c r="G105" t="s">
-        <v>27</v>
+        <v>168</v>
       </c>
       <c r="H105" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I105" s="1">
         <f>VLOOKUP(F105,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G105,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H105,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B106" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C106" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="F106" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G106" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H106" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I106" s="1">
         <f>VLOOKUP(F106,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G106,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H106,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>6.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B107" t="s">
         <v>67</v>
@@ -6162,31 +6170,31 @@
         <v>74</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F107" t="s">
         <v>16</v>
       </c>
       <c r="G107" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H107" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="I107" s="1">
         <f>VLOOKUP(F107,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G107,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H107,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>1.5</v>
-      </c>
-      <c r="J107">
-        <v>27</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B108" t="s">
-        <v>39</v>
+        <v>67</v>
+      </c>
+      <c r="C108" t="s">
+        <v>74</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>80</v>
@@ -6210,16 +6218,13 @@
     </row>
     <row r="109" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B109" t="s">
-        <v>76</v>
-      </c>
-      <c r="C109" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F109" t="s">
         <v>16</v>
@@ -6228,17 +6233,47 @@
         <v>30</v>
       </c>
       <c r="H109" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="I109" s="1">
         <f>VLOOKUP(F109,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G109,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H109,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J109">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>27</v>
+      </c>
+      <c r="B110" t="s">
+        <v>76</v>
+      </c>
+      <c r="C110" t="s">
+        <v>77</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F110" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" t="s">
+        <v>30</v>
+      </c>
+      <c r="H110" t="s">
+        <v>70</v>
+      </c>
+      <c r="I110" s="1">
+        <f>VLOOKUP(F110,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G110,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H110,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>0.42857142857142855</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K109">
-      <sortCondition descending="1" ref="I1:I109"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K110">
+      <sortCondition descending="1" ref="I1:I110"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
e-Questrain: Minor fixes to UI
</commit_message>
<xml_diff>
--- a/e-Question - To do list.xlsx
+++ b/e-Question - To do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B1D08E-8219-9F46-A293-C5FB02144C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8365D22-B27C-3645-9544-DF730721D39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of completion" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="210">
   <si>
     <t>Sections</t>
   </si>
@@ -699,6 +699,15 @@
   </si>
   <si>
     <t>Sum of Priority S</t>
+  </si>
+  <si>
+    <t>Login/Register</t>
+  </si>
+  <si>
+    <t>Register modal</t>
+  </si>
+  <si>
+    <t>Needs to be a modal specfically for modals</t>
   </si>
 </sst>
 </file>
@@ -774,29 +783,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -810,13 +797,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45300.478778124998" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="114" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45307.43574976852" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="114" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:M1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
   <cacheFields count="13">
     <cacheField name="#" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="112"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="113"/>
     </cacheField>
     <cacheField name="Section" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -896,7 +883,7 @@
     <n v="7"/>
     <n v="98"/>
     <n v="1"/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="77"/>
@@ -974,6 +961,21 @@
     <x v="0"/>
   </r>
   <r>
+    <n v="113"/>
+    <s v="Login/Register"/>
+    <s v="Register modal"/>
+    <m/>
+    <s v="Needs to be a modal specfically for modals"/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="New component/service with simple integration"/>
+    <n v="8"/>
+    <n v="6"/>
+    <n v="57.6"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
     <n v="25"/>
     <s v="User Management"/>
     <s v="Sign in Modal"/>
@@ -1094,7 +1096,7 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="3"/>
+    <n v="17"/>
     <s v="Marketing"/>
     <s v="Landing Page"/>
     <s v="What's New Section"/>
@@ -2563,26 +2565,11 @@
     <m/>
     <x v="1"/>
   </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:D15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2638,7 +2625,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2694,7 +2681,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -3048,13 +3035,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CCC35A-14FA-1E40-8319-0349AC17C33D}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3080,19 +3067,19 @@
         <v>206</v>
       </c>
       <c r="B3" s="8">
-        <v>651</v>
+        <v>749</v>
       </c>
       <c r="C3" s="8">
-        <v>2318.9976190476186</v>
+        <v>2278.5976190476185</v>
       </c>
       <c r="D3" s="8">
-        <v>2969.9976190476186</v>
+        <v>3027.5976190476185</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="7">
         <f>GETPIVOTDATA("Priority S",$A$1,"Status","Done")/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.21919209491109104</v>
+        <v>0.24739086703193092</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3116,19 +3103,19 @@
         <v>183</v>
       </c>
       <c r="B9" s="8">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C9" s="8">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D9" s="8">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="7">
         <f>GETPIVOTDATA("Importance S",$A$7,"Status","Done")/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.15229885057471265</v>
+        <v>0.1601123595505618</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3152,19 +3139,19 @@
         <v>184</v>
       </c>
       <c r="B15" s="8">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C15" s="8">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D15" s="8">
-        <v>651</v>
+        <v>657</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="7">
         <f>GETPIVOTDATA("Impact S",$A$13,"Status","Done")/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>6.6052227342549924E-2</v>
+        <v>7.6103500761035003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3174,10 +3161,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDA03E2-CB53-DC47-9991-2200F2AD06AB}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3485,6 +3472,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>207</v>
+      </c>
       <c r="B16" t="s">
         <v>73</v>
       </c>
@@ -3573,6 +3563,11 @@
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3585,10 +3580,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
-  <dimension ref="A1:M113"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3597,13 +3592,13 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.83203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3693,42 +3688,45 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="5">
         <f>VLOOKUP(F3,'Source lists'!$E$1:F7,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="5">
         <f>VLOOKUP(G3,'Source lists'!$H$1:I8,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="5">
         <f>VLOOKUP(F3,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G3,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H3,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>98</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>1</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3892,7 +3890,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>32</v>
       </c>
@@ -3934,94 +3932,91 @@
     </row>
     <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="1">
+        <f>VLOOKUP(F9,'Source lists'!$E$1:F118,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="J9" s="1">
+        <f>VLOOKUP(G9,'Source lists'!$H$1:I119,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="K9" s="1">
+        <f>VLOOKUP(F9,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G9,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H9,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>57.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="5">
-        <f>VLOOKUP(F9,'Source lists'!$E$1:F12,2,FALSE)</f>
+      <c r="I10" s="5">
+        <f>VLOOKUP(F10,'Source lists'!$E$1:F12,2,FALSE)</f>
         <v>10</v>
       </c>
-      <c r="J9" s="5">
-        <f>VLOOKUP(G9,'Source lists'!$H$1:I13,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="K9" s="5">
-        <f>VLOOKUP(F9,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G9,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H9,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+      <c r="J10" s="5">
+        <f>VLOOKUP(G10,'Source lists'!$H$1:I13,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="K10" s="5">
+        <f>VLOOKUP(F10,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G10,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H10,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>53.333333333333336</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3" t="s">
+      <c r="L10" s="3"/>
+      <c r="M10" s="3" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="1">
-        <f>VLOOKUP(F10,'Source lists'!$E$1:F13,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J10" s="1">
-        <f>VLOOKUP(G10,'Source lists'!$H$1:I14,2,FALSE)</f>
-        <v>10</v>
-      </c>
-      <c r="K10" s="1">
-        <f>VLOOKUP(F10,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G10,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H10,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>50</v>
-      </c>
-      <c r="L10">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -4033,11 +4028,11 @@
         <v>23</v>
       </c>
       <c r="I11" s="1">
-        <f>VLOOKUP(F11,'Source lists'!$E$1:F14,2,FALSE)</f>
+        <f>VLOOKUP(F11,'Source lists'!$E$1:F13,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J11" s="1">
-        <f>VLOOKUP(G11,'Source lists'!$H$1:I15,2,FALSE)</f>
+        <f>VLOOKUP(G11,'Source lists'!$H$1:I14,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K11" s="1">
@@ -4045,12 +4040,12 @@
         <v>50</v>
       </c>
       <c r="L11">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -4059,7 +4054,7 @@
         <v>91</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -4071,11 +4066,11 @@
         <v>23</v>
       </c>
       <c r="I12" s="1">
-        <f>VLOOKUP(F12,'Source lists'!$E$1:F15,2,FALSE)</f>
+        <f>VLOOKUP(F12,'Source lists'!$E$1:F14,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J12" s="1">
-        <f>VLOOKUP(G12,'Source lists'!$H$1:I16,2,FALSE)</f>
+        <f>VLOOKUP(G12,'Source lists'!$H$1:I15,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K12" s="1">
@@ -4083,22 +4078,22 @@
         <v>50</v>
       </c>
       <c r="L12">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -4110,11 +4105,11 @@
         <v>23</v>
       </c>
       <c r="I13" s="1">
-        <f>VLOOKUP(F13,'Source lists'!$E$1:F16,2,FALSE)</f>
+        <f>VLOOKUP(F13,'Source lists'!$E$1:F15,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J13" s="1">
-        <f>VLOOKUP(G13,'Source lists'!$H$1:I17,2,FALSE)</f>
+        <f>VLOOKUP(G13,'Source lists'!$H$1:I16,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K13" s="1">
@@ -4122,91 +4117,91 @@
         <v>50</v>
       </c>
       <c r="L13">
+        <v>63</v>
+      </c>
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="1">
+        <f>VLOOKUP(F14,'Source lists'!$E$1:F16,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <f>VLOOKUP(G14,'Source lists'!$H$1:I17,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="K14" s="1">
+        <f>VLOOKUP(F14,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G14,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H14,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="L14">
         <v>61</v>
       </c>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="5">
-        <f>VLOOKUP(F14,'Source lists'!$E$1:F17,2,FALSE)</f>
+      <c r="I15" s="5">
+        <f>VLOOKUP(F15,'Source lists'!$E$1:F17,2,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="J14" s="5">
-        <f>VLOOKUP(G14,'Source lists'!$H$1:I18,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="K14" s="5">
-        <f>VLOOKUP(F14,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G14,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H14,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+      <c r="J15" s="5">
+        <f>VLOOKUP(G15,'Source lists'!$H$1:I18,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="K15" s="5">
+        <f>VLOOKUP(F15,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G15,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H15,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>42.666666666666664</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3" t="s">
+      <c r="L15" s="3"/>
+      <c r="M15" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="1">
-        <f>VLOOKUP(F15,'Source lists'!$E$1:F18,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="J15" s="1">
-        <f>VLOOKUP(G15,'Source lists'!$H$1:I19,2,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="K15" s="1">
-        <f>VLOOKUP(F15,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G15,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H15,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>39.200000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
@@ -4215,10 +4210,10 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
@@ -4230,11 +4225,11 @@
         <v>70</v>
       </c>
       <c r="I16" s="1">
-        <f>VLOOKUP(F16,'Source lists'!$E$1:F19,2,FALSE)</f>
+        <f>VLOOKUP(F16,'Source lists'!$E$1:F18,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J16" s="1">
-        <f>VLOOKUP(G16,'Source lists'!$H$1:I20,2,FALSE)</f>
+        <f>VLOOKUP(G16,'Source lists'!$H$1:I19,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K16" s="1">
@@ -4244,7 +4239,7 @@
     </row>
     <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
@@ -4253,7 +4248,7 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>95</v>
@@ -4268,11 +4263,11 @@
         <v>70</v>
       </c>
       <c r="I17" s="1">
-        <f>VLOOKUP(F17,'Source lists'!$E$1:F20,2,FALSE)</f>
+        <f>VLOOKUP(F17,'Source lists'!$E$1:F19,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J17" s="1">
-        <f>VLOOKUP(G17,'Source lists'!$H$1:I21,2,FALSE)</f>
+        <f>VLOOKUP(G17,'Source lists'!$H$1:I20,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K17" s="1">
@@ -4282,7 +4277,8 @@
     </row>
     <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>4</v>
+        <f>A57</f>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -4291,7 +4287,7 @@
         <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>95</v>
@@ -4306,11 +4302,11 @@
         <v>70</v>
       </c>
       <c r="I18" s="1">
-        <f>VLOOKUP(F18,'Source lists'!$E$1:F21,2,FALSE)</f>
+        <f>VLOOKUP(F18,'Source lists'!$E$1:F20,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J18" s="1">
-        <f>VLOOKUP(G18,'Source lists'!$H$1:I22,2,FALSE)</f>
+        <f>VLOOKUP(G18,'Source lists'!$H$1:I21,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K18" s="1">
@@ -4318,9 +4314,9 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>39</v>
@@ -4329,7 +4325,7 @@
         <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>95</v>
@@ -4344,11 +4340,11 @@
         <v>70</v>
       </c>
       <c r="I19" s="1">
-        <f>VLOOKUP(F19,'Source lists'!$E$1:F22,2,FALSE)</f>
+        <f>VLOOKUP(F19,'Source lists'!$E$1:F21,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J19" s="1">
-        <f>VLOOKUP(G19,'Source lists'!$H$1:I23,2,FALSE)</f>
+        <f>VLOOKUP(G19,'Source lists'!$H$1:I22,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K19" s="1">
@@ -4358,19 +4354,19 @@
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="F20" t="s">
         <v>15</v>
@@ -4382,11 +4378,11 @@
         <v>70</v>
       </c>
       <c r="I20" s="1">
-        <f>VLOOKUP(F20,'Source lists'!$E$1:F23,2,FALSE)</f>
+        <f>VLOOKUP(F20,'Source lists'!$E$1:F22,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J20" s="1">
-        <f>VLOOKUP(G20,'Source lists'!$H$1:I24,2,FALSE)</f>
+        <f>VLOOKUP(G20,'Source lists'!$H$1:I23,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K20" s="1">
@@ -4394,9 +4390,9 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -4404,34 +4400,37 @@
       <c r="C21" t="s">
         <v>42</v>
       </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
       <c r="E21" s="2" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I21" s="1">
-        <f>VLOOKUP(F21,'Source lists'!$E$1:F24,2,FALSE)</f>
+        <f>VLOOKUP(F21,'Source lists'!$E$1:F23,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J21" s="1">
-        <f>VLOOKUP(G21,'Source lists'!$H$1:I25,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G21,'Source lists'!$H$1:I24,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K21" s="1">
         <f>VLOOKUP(F21,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G21,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H21,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -4439,11 +4438,8 @@
       <c r="C22" t="s">
         <v>42</v>
       </c>
-      <c r="D22" t="s">
-        <v>44</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
@@ -4455,24 +4451,21 @@
         <v>23</v>
       </c>
       <c r="I22" s="1">
-        <f>VLOOKUP(F22,'Source lists'!$E$1:F25,2,FALSE)</f>
+        <f>VLOOKUP(F22,'Source lists'!$E$1:F24,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J22" s="1">
-        <f>VLOOKUP(G22,'Source lists'!$H$1:I26,2,FALSE)</f>
+        <f>VLOOKUP(G22,'Source lists'!$H$1:I25,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K22" s="1">
         <f>VLOOKUP(F22,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G22,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H22,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L22">
-        <v>8</v>
-      </c>
     </row>
     <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -4484,7 +4477,7 @@
         <v>44</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
@@ -4496,11 +4489,11 @@
         <v>23</v>
       </c>
       <c r="I23" s="1">
-        <f>VLOOKUP(F23,'Source lists'!$E$1:F26,2,FALSE)</f>
+        <f>VLOOKUP(F23,'Source lists'!$E$1:F25,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J23" s="1">
-        <f>VLOOKUP(G23,'Source lists'!$H$1:I27,2,FALSE)</f>
+        <f>VLOOKUP(G23,'Source lists'!$H$1:I26,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K23" s="1">
@@ -4513,7 +4506,7 @@
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -4525,7 +4518,7 @@
         <v>44</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
@@ -4537,11 +4530,11 @@
         <v>23</v>
       </c>
       <c r="I24" s="1">
-        <f>VLOOKUP(F24,'Source lists'!$E$1:F27,2,FALSE)</f>
+        <f>VLOOKUP(F24,'Source lists'!$E$1:F26,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J24" s="1">
-        <f>VLOOKUP(G24,'Source lists'!$H$1:I28,2,FALSE)</f>
+        <f>VLOOKUP(G24,'Source lists'!$H$1:I27,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K24" s="1">
@@ -4554,7 +4547,7 @@
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -4566,7 +4559,7 @@
         <v>44</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
@@ -4578,11 +4571,11 @@
         <v>23</v>
       </c>
       <c r="I25" s="1">
-        <f>VLOOKUP(F25,'Source lists'!$E$1:F28,2,FALSE)</f>
+        <f>VLOOKUP(F25,'Source lists'!$E$1:F27,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J25" s="1">
-        <f>VLOOKUP(G25,'Source lists'!$H$1:I29,2,FALSE)</f>
+        <f>VLOOKUP(G25,'Source lists'!$H$1:I28,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K25" s="1">
@@ -4595,7 +4588,7 @@
     </row>
     <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -4607,7 +4600,7 @@
         <v>44</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -4619,11 +4612,11 @@
         <v>23</v>
       </c>
       <c r="I26" s="1">
-        <f>VLOOKUP(F26,'Source lists'!$E$1:F29,2,FALSE)</f>
+        <f>VLOOKUP(F26,'Source lists'!$E$1:F28,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J26" s="1">
-        <f>VLOOKUP(G26,'Source lists'!$H$1:I30,2,FALSE)</f>
+        <f>VLOOKUP(G26,'Source lists'!$H$1:I29,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K26" s="1">
@@ -4636,7 +4629,7 @@
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -4648,7 +4641,7 @@
         <v>44</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -4660,11 +4653,11 @@
         <v>23</v>
       </c>
       <c r="I27" s="1">
-        <f>VLOOKUP(F27,'Source lists'!$E$1:F30,2,FALSE)</f>
+        <f>VLOOKUP(F27,'Source lists'!$E$1:F29,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J27" s="1">
-        <f>VLOOKUP(G27,'Source lists'!$H$1:I31,2,FALSE)</f>
+        <f>VLOOKUP(G27,'Source lists'!$H$1:I30,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K27" s="1">
@@ -4677,7 +4670,7 @@
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -4689,7 +4682,7 @@
         <v>44</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
@@ -4701,11 +4694,11 @@
         <v>23</v>
       </c>
       <c r="I28" s="1">
-        <f>VLOOKUP(F28,'Source lists'!$E$1:F31,2,FALSE)</f>
+        <f>VLOOKUP(F28,'Source lists'!$E$1:F30,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J28" s="1">
-        <f>VLOOKUP(G28,'Source lists'!$H$1:I32,2,FALSE)</f>
+        <f>VLOOKUP(G28,'Source lists'!$H$1:I31,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K28" s="1">
@@ -4718,7 +4711,7 @@
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -4730,7 +4723,7 @@
         <v>44</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
@@ -4742,11 +4735,11 @@
         <v>23</v>
       </c>
       <c r="I29" s="1">
-        <f>VLOOKUP(F29,'Source lists'!$E$1:F32,2,FALSE)</f>
+        <f>VLOOKUP(F29,'Source lists'!$E$1:F31,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J29" s="1">
-        <f>VLOOKUP(G29,'Source lists'!$H$1:I33,2,FALSE)</f>
+        <f>VLOOKUP(G29,'Source lists'!$H$1:I32,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K29" s="1">
@@ -4759,7 +4752,7 @@
     </row>
     <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -4768,10 +4761,10 @@
         <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -4783,30 +4776,36 @@
         <v>23</v>
       </c>
       <c r="I30" s="1">
-        <f>VLOOKUP(F30,'Source lists'!$E$1:F33,2,FALSE)</f>
+        <f>VLOOKUP(F30,'Source lists'!$E$1:F32,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J30" s="1">
-        <f>VLOOKUP(G30,'Source lists'!$H$1:I34,2,FALSE)</f>
+        <f>VLOOKUP(G30,'Source lists'!$H$1:I33,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K30" s="1">
         <f>VLOOKUP(F30,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G30,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H30,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="L30">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="F31" t="s">
         <v>15</v>
@@ -4818,11 +4817,11 @@
         <v>23</v>
       </c>
       <c r="I31" s="1">
-        <f>VLOOKUP(F31,'Source lists'!$E$1:F34,2,FALSE)</f>
+        <f>VLOOKUP(F31,'Source lists'!$E$1:F33,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J31" s="1">
-        <f>VLOOKUP(G31,'Source lists'!$H$1:I35,2,FALSE)</f>
+        <f>VLOOKUP(G31,'Source lists'!$H$1:I34,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K31" s="1">
@@ -4832,7 +4831,7 @@
     </row>
     <row r="32" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>38</v>
@@ -4840,11 +4839,8 @@
       <c r="C32" t="s">
         <v>80</v>
       </c>
-      <c r="D32" t="s">
-        <v>85</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
@@ -4856,11 +4852,11 @@
         <v>23</v>
       </c>
       <c r="I32" s="1">
-        <f>VLOOKUP(F32,'Source lists'!$E$1:F35,2,FALSE)</f>
+        <f>VLOOKUP(F32,'Source lists'!$E$1:F34,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J32" s="1">
-        <f>VLOOKUP(G32,'Source lists'!$H$1:I36,2,FALSE)</f>
+        <f>VLOOKUP(G32,'Source lists'!$H$1:I35,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K32" s="1">
@@ -4868,18 +4864,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="D33" t="s">
+        <v>85</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -4891,11 +4890,11 @@
         <v>23</v>
       </c>
       <c r="I33" s="1">
-        <f>VLOOKUP(F33,'Source lists'!$E$1:F36,2,FALSE)</f>
+        <f>VLOOKUP(F33,'Source lists'!$E$1:F35,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J33" s="1">
-        <f>VLOOKUP(G33,'Source lists'!$H$1:I37,2,FALSE)</f>
+        <f>VLOOKUP(G33,'Source lists'!$H$1:I36,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K33" s="1">
@@ -4903,18 +4902,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
@@ -4926,11 +4925,11 @@
         <v>23</v>
       </c>
       <c r="I34" s="1">
-        <f>VLOOKUP(F34,'Source lists'!$E$1:F37,2,FALSE)</f>
+        <f>VLOOKUP(F34,'Source lists'!$E$1:F36,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J34" s="1">
-        <f>VLOOKUP(G34,'Source lists'!$H$1:I38,2,FALSE)</f>
+        <f>VLOOKUP(G34,'Source lists'!$H$1:I37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K34" s="1">
@@ -4938,18 +4937,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F35" t="s">
         <v>15</v>
@@ -4961,11 +4960,11 @@
         <v>23</v>
       </c>
       <c r="I35" s="1">
-        <f>VLOOKUP(F35,'Source lists'!$E$1:F38,2,FALSE)</f>
+        <f>VLOOKUP(F35,'Source lists'!$E$1:F37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J35" s="1">
-        <f>VLOOKUP(G35,'Source lists'!$H$1:I39,2,FALSE)</f>
+        <f>VLOOKUP(G35,'Source lists'!$H$1:I38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K35" s="1">
@@ -4973,9 +4972,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -4984,7 +4983,7 @@
         <v>106</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -4996,11 +4995,11 @@
         <v>23</v>
       </c>
       <c r="I36" s="1">
-        <f>VLOOKUP(F36,'Source lists'!$E$1:F39,2,FALSE)</f>
+        <f>VLOOKUP(F36,'Source lists'!$E$1:F38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J36" s="1">
-        <f>VLOOKUP(G36,'Source lists'!$H$1:I40,2,FALSE)</f>
+        <f>VLOOKUP(G36,'Source lists'!$H$1:I39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K36" s="1">
@@ -5008,18 +5007,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -5031,11 +5030,11 @@
         <v>23</v>
       </c>
       <c r="I37" s="1">
-        <f>VLOOKUP(F37,'Source lists'!$E$1:F40,2,FALSE)</f>
+        <f>VLOOKUP(F37,'Source lists'!$E$1:F39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J37" s="1">
-        <f>VLOOKUP(G37,'Source lists'!$H$1:I41,2,FALSE)</f>
+        <f>VLOOKUP(G37,'Source lists'!$H$1:I40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K37" s="1">
@@ -5043,9 +5042,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -5054,7 +5053,7 @@
         <v>150</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
@@ -5066,11 +5065,11 @@
         <v>23</v>
       </c>
       <c r="I38" s="1">
-        <f>VLOOKUP(F38,'Source lists'!$E$1:F41,2,FALSE)</f>
+        <f>VLOOKUP(F38,'Source lists'!$E$1:F40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J38" s="1">
-        <f>VLOOKUP(G38,'Source lists'!$H$1:I42,2,FALSE)</f>
+        <f>VLOOKUP(G38,'Source lists'!$H$1:I41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K38" s="1">
@@ -5078,18 +5077,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="F39" t="s">
         <v>15</v>
@@ -5101,11 +5100,11 @@
         <v>23</v>
       </c>
       <c r="I39" s="1">
-        <f>VLOOKUP(F39,'Source lists'!$E$1:F42,2,FALSE)</f>
+        <f>VLOOKUP(F39,'Source lists'!$E$1:F41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J39" s="1">
-        <f>VLOOKUP(G39,'Source lists'!$H$1:I43,2,FALSE)</f>
+        <f>VLOOKUP(G39,'Source lists'!$H$1:I42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K39" s="1">
@@ -5113,18 +5112,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
@@ -5136,11 +5135,11 @@
         <v>23</v>
       </c>
       <c r="I40" s="1">
-        <f>VLOOKUP(F40,'Source lists'!$E$1:F43,2,FALSE)</f>
+        <f>VLOOKUP(F40,'Source lists'!$E$1:F42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J40" s="1">
-        <f>VLOOKUP(G40,'Source lists'!$H$1:I44,2,FALSE)</f>
+        <f>VLOOKUP(G40,'Source lists'!$H$1:I43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K40" s="1">
@@ -5148,21 +5147,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" t="s">
-        <v>180</v>
+        <v>150</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="F41" t="s">
         <v>15</v>
@@ -5174,24 +5170,21 @@
         <v>23</v>
       </c>
       <c r="I41" s="1">
-        <f>VLOOKUP(F41,'Source lists'!$E$1:F44,2,FALSE)</f>
+        <f>VLOOKUP(F41,'Source lists'!$E$1:F43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J41" s="1">
-        <f>VLOOKUP(G41,'Source lists'!$H$1:I45,2,FALSE)</f>
+        <f>VLOOKUP(G41,'Source lists'!$H$1:I44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K41" s="1">
         <f>VLOOKUP(F41,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G41,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H41,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L41">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -5203,33 +5196,36 @@
         <v>44</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>46</v>
+        <v>180</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H42" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="I42" s="1">
-        <f>VLOOKUP(F42,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <f>VLOOKUP(F42,'Source lists'!$E$1:F44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J42" s="1">
-        <f>VLOOKUP(G42,'Source lists'!$H$1:I46,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(G42,'Source lists'!$H$1:I45,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K42" s="1">
         <f>VLOOKUP(F42,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G42,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H42,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="L42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -5237,69 +5233,72 @@
       <c r="C43" t="s">
         <v>42</v>
       </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
       <c r="E43" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G43" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H43" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="I43" s="1">
-        <f>VLOOKUP(F43,'Source lists'!$E$1:F46,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F43,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J43" s="1">
-        <f>VLOOKUP(G43,'Source lists'!$H$1:I47,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G43,'Source lists'!$H$1:I46,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K43" s="1">
         <f>VLOOKUP(F43,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G43,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H43,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="F44" t="s">
         <v>16</v>
       </c>
       <c r="G44" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="H44" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="I44" s="1">
-        <f>VLOOKUP(F44,'Source lists'!$E$1:F47,2,FALSE)</f>
+        <f>VLOOKUP(F44,'Source lists'!$E$1:F46,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J44" s="1">
-        <f>VLOOKUP(G44,'Source lists'!$H$1:I48,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G44,'Source lists'!$H$1:I47,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K44" s="1">
         <f>VLOOKUP(F44,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G44,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H44,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -5308,7 +5307,7 @@
         <v>87</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F45" t="s">
         <v>16</v>
@@ -5320,11 +5319,11 @@
         <v>67</v>
       </c>
       <c r="I45" s="1">
-        <f>VLOOKUP(F45,'Source lists'!$E$1:F48,2,FALSE)</f>
+        <f>VLOOKUP(F45,'Source lists'!$E$1:F47,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J45" s="1">
-        <f>VLOOKUP(G45,'Source lists'!$H$1:I49,2,FALSE)</f>
+        <f>VLOOKUP(G45,'Source lists'!$H$1:I48,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K45" s="1">
@@ -5332,53 +5331,53 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F46" t="s">
         <v>16</v>
       </c>
       <c r="G46" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="H46" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="I46" s="1">
-        <f>VLOOKUP(F46,'Source lists'!$E$1:F49,2,FALSE)</f>
+        <f>VLOOKUP(F46,'Source lists'!$E$1:F48,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J46" s="1">
-        <f>VLOOKUP(G46,'Source lists'!$H$1:I50,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G46,'Source lists'!$H$1:I49,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K46" s="1">
         <f>VLOOKUP(F46,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G46,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H46,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F47" t="s">
         <v>16</v>
@@ -5390,11 +5389,11 @@
         <v>25</v>
       </c>
       <c r="I47" s="1">
-        <f>VLOOKUP(F47,'Source lists'!$E$1:F50,2,FALSE)</f>
+        <f>VLOOKUP(F47,'Source lists'!$E$1:F49,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J47" s="1">
-        <f>VLOOKUP(G47,'Source lists'!$H$1:I51,2,FALSE)</f>
+        <f>VLOOKUP(G47,'Source lists'!$H$1:I50,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K47" s="1">
@@ -5402,94 +5401,91 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
+    <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>57</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="F48" s="3" t="s">
+      <c r="E48" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" t="s">
         <v>16</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G48" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" t="s">
         <v>25</v>
       </c>
-      <c r="I48" s="5">
-        <f>VLOOKUP(F48,'Source lists'!$E$1:F51,2,FALSE)</f>
+      <c r="I48" s="1">
+        <f>VLOOKUP(F48,'Source lists'!$E$1:F50,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="J48" s="5">
-        <f>VLOOKUP(G48,'Source lists'!$H$1:I52,2,FALSE)</f>
+      <c r="J48" s="1">
+        <f>VLOOKUP(G48,'Source lists'!$H$1:I51,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="K48" s="5">
+      <c r="K48" s="1">
         <f>VLOOKUP(F48,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G48,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H48,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3" t="s">
+    </row>
+    <row r="49" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>106</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I49" s="5">
+        <f>VLOOKUP(F49,'Source lists'!$E$1:F51,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="J49" s="5">
+        <f>VLOOKUP(G49,'Source lists'!$H$1:I52,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="K49" s="5">
+        <f>VLOOKUP(F49,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G49,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H49,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49">
+    <row r="50" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>1</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>91</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="F49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" t="s">
-        <v>28</v>
-      </c>
-      <c r="H49" t="s">
-        <v>24</v>
-      </c>
-      <c r="I49" s="1">
-        <f>VLOOKUP(F49,'Source lists'!$E$1:F52,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="J49" s="1">
-        <f>VLOOKUP(G49,'Source lists'!$H$1:I53,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="K49" s="1">
-        <f>VLOOKUP(F49,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G49,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H49,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>21.333333333333332</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>74</v>
-      </c>
-      <c r="B50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" t="s">
-        <v>133</v>
-      </c>
-      <c r="D50" t="s">
-        <v>188</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
@@ -5501,11 +5497,11 @@
         <v>24</v>
       </c>
       <c r="I50" s="1">
-        <f>VLOOKUP(F50,'Source lists'!$E$1:F53,2,FALSE)</f>
+        <f>VLOOKUP(F50,'Source lists'!$E$1:F52,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J50" s="1">
-        <f>VLOOKUP(G50,'Source lists'!$H$1:I54,2,FALSE)</f>
+        <f>VLOOKUP(G50,'Source lists'!$H$1:I53,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K50" s="1">
@@ -5513,18 +5509,21 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="D51" t="s">
+        <v>188</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="F51" t="s">
         <v>15</v>
@@ -5536,11 +5535,11 @@
         <v>24</v>
       </c>
       <c r="I51" s="1">
-        <f>VLOOKUP(F51,'Source lists'!$E$1:F54,2,FALSE)</f>
+        <f>VLOOKUP(F51,'Source lists'!$E$1:F53,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J51" s="1">
-        <f>VLOOKUP(G51,'Source lists'!$H$1:I55,2,FALSE)</f>
+        <f>VLOOKUP(G51,'Source lists'!$H$1:I54,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K51" s="1">
@@ -5548,18 +5547,18 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="F52" t="s">
         <v>15</v>
@@ -5571,11 +5570,11 @@
         <v>24</v>
       </c>
       <c r="I52" s="1">
-        <f>VLOOKUP(F52,'Source lists'!$E$1:F55,2,FALSE)</f>
+        <f>VLOOKUP(F52,'Source lists'!$E$1:F54,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J52" s="1">
-        <f>VLOOKUP(G52,'Source lists'!$H$1:I56,2,FALSE)</f>
+        <f>VLOOKUP(G52,'Source lists'!$H$1:I55,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K52" s="1">
@@ -5583,18 +5582,18 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -5606,11 +5605,11 @@
         <v>24</v>
       </c>
       <c r="I53" s="1">
-        <f>VLOOKUP(F53,'Source lists'!$E$1:F56,2,FALSE)</f>
+        <f>VLOOKUP(F53,'Source lists'!$E$1:F55,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J53" s="1">
-        <f>VLOOKUP(G53,'Source lists'!$H$1:I57,2,FALSE)</f>
+        <f>VLOOKUP(G53,'Source lists'!$H$1:I56,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K53" s="1">
@@ -5618,18 +5617,18 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
@@ -5641,11 +5640,11 @@
         <v>24</v>
       </c>
       <c r="I54" s="1">
-        <f>VLOOKUP(F54,'Source lists'!$E$1:F57,2,FALSE)</f>
+        <f>VLOOKUP(F54,'Source lists'!$E$1:F56,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J54" s="1">
-        <f>VLOOKUP(G54,'Source lists'!$H$1:I58,2,FALSE)</f>
+        <f>VLOOKUP(G54,'Source lists'!$H$1:I57,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K54" s="1">
@@ -5653,9 +5652,9 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
@@ -5664,7 +5663,7 @@
         <v>154</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
@@ -5676,11 +5675,11 @@
         <v>24</v>
       </c>
       <c r="I55" s="1">
-        <f>VLOOKUP(F55,'Source lists'!$E$1:F58,2,FALSE)</f>
+        <f>VLOOKUP(F55,'Source lists'!$E$1:F57,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J55" s="1">
-        <f>VLOOKUP(G55,'Source lists'!$H$1:I59,2,FALSE)</f>
+        <f>VLOOKUP(G55,'Source lists'!$H$1:I58,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K55" s="1">
@@ -5688,47 +5687,44 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
       </c>
       <c r="G56" t="s">
-        <v>159</v>
+        <v>28</v>
       </c>
       <c r="H56" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="I56" s="1">
-        <f>VLOOKUP(F56,'Source lists'!$E$1:F59,2,FALSE)</f>
+        <f>VLOOKUP(F56,'Source lists'!$E$1:F58,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J56" s="1">
-        <f>VLOOKUP(G56,'Source lists'!$H$1:I60,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G56,'Source lists'!$H$1:I59,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K56" s="1">
         <f>VLOOKUP(F56,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G56,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H56,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>20.571428571428573</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>21.333333333333332</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -5740,7 +5736,7 @@
         <v>54</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
@@ -5752,11 +5748,11 @@
         <v>69</v>
       </c>
       <c r="I57" s="1">
-        <f>VLOOKUP(F57,'Source lists'!$E$1:F60,2,FALSE)</f>
+        <f>VLOOKUP(F57,'Source lists'!$E$1:F59,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J57" s="1">
-        <f>VLOOKUP(G57,'Source lists'!$H$1:I61,2,FALSE)</f>
+        <f>VLOOKUP(G57,'Source lists'!$H$1:I60,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K57" s="1">
@@ -5764,9 +5760,9 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -5778,7 +5774,7 @@
         <v>54</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -5790,11 +5786,11 @@
         <v>69</v>
       </c>
       <c r="I58" s="1">
-        <f>VLOOKUP(F58,'Source lists'!$E$1:F61,2,FALSE)</f>
+        <f>VLOOKUP(F58,'Source lists'!$E$1:F60,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J58" s="1">
-        <f>VLOOKUP(G58,'Source lists'!$H$1:I62,2,FALSE)</f>
+        <f>VLOOKUP(G58,'Source lists'!$H$1:I61,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K58" s="1">
@@ -5802,9 +5798,9 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -5816,7 +5812,7 @@
         <v>54</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F59" t="s">
         <v>15</v>
@@ -5828,11 +5824,11 @@
         <v>69</v>
       </c>
       <c r="I59" s="1">
-        <f>VLOOKUP(F59,'Source lists'!$E$1:F62,2,FALSE)</f>
+        <f>VLOOKUP(F59,'Source lists'!$E$1:F61,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J59" s="1">
-        <f>VLOOKUP(G59,'Source lists'!$H$1:I63,2,FALSE)</f>
+        <f>VLOOKUP(G59,'Source lists'!$H$1:I62,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K59" s="1">
@@ -5840,9 +5836,9 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
@@ -5854,7 +5850,7 @@
         <v>54</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F60" t="s">
         <v>15</v>
@@ -5866,11 +5862,11 @@
         <v>69</v>
       </c>
       <c r="I60" s="1">
-        <f>VLOOKUP(F60,'Source lists'!$E$1:F63,2,FALSE)</f>
+        <f>VLOOKUP(F60,'Source lists'!$E$1:F62,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J60" s="1">
-        <f>VLOOKUP(G60,'Source lists'!$H$1:I64,2,FALSE)</f>
+        <f>VLOOKUP(G60,'Source lists'!$H$1:I63,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K60" s="1">
@@ -5878,53 +5874,56 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>106</v>
+        <v>42</v>
+      </c>
+      <c r="D61" t="s">
+        <v>54</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>190</v>
+        <v>60</v>
       </c>
       <c r="F61" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G61" t="s">
         <v>159</v>
       </c>
       <c r="H61" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="I61" s="1">
-        <f>VLOOKUP(F61,'Source lists'!$E$1:F64,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F61,'Source lists'!$E$1:F63,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J61" s="1">
-        <f>VLOOKUP(G61,'Source lists'!$H$1:I65,2,FALSE)</f>
+        <f>VLOOKUP(G61,'Source lists'!$H$1:I64,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K61" s="1">
         <f>VLOOKUP(F61,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G61,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H61,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>20.571428571428573</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>141</v>
+        <v>190</v>
       </c>
       <c r="F62" t="s">
         <v>17</v>
@@ -5936,11 +5935,11 @@
         <v>23</v>
       </c>
       <c r="I62" s="1">
-        <f>VLOOKUP(F62,'Source lists'!$E$1:F65,2,FALSE)</f>
+        <f>VLOOKUP(F62,'Source lists'!$E$1:F64,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J62" s="1">
-        <f>VLOOKUP(G62,'Source lists'!$H$1:I66,2,FALSE)</f>
+        <f>VLOOKUP(G62,'Source lists'!$H$1:I65,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K62" s="1">
@@ -5948,91 +5947,88 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>133</v>
-      </c>
-      <c r="D63" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F63" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G63" t="s">
-        <v>28</v>
+        <v>159</v>
       </c>
       <c r="H63" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="I63" s="1">
-        <f>VLOOKUP(F63,'Source lists'!$E$1:F66,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F63,'Source lists'!$E$1:F65,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J63" s="1">
-        <f>VLOOKUP(G63,'Source lists'!$H$1:I67,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G63,'Source lists'!$H$1:I66,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K63" s="1">
         <f>VLOOKUP(F63,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G63,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H63,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>161</v>
+        <v>133</v>
+      </c>
+      <c r="D64" t="s">
+        <v>188</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="F64" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G64" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I64" s="1">
-        <f>VLOOKUP(F64,'Source lists'!$E$1:F67,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F64,'Source lists'!$E$1:F66,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J64" s="1">
-        <f>VLOOKUP(G64,'Source lists'!$H$1:I68,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(G64,'Source lists'!$H$1:I67,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K64" s="1">
         <f>VLOOKUP(F64,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G64,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H64,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="L64">
-        <v>59</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>167</v>
@@ -6047,11 +6043,11 @@
         <v>69</v>
       </c>
       <c r="I65" s="1">
-        <f>VLOOKUP(F65,'Source lists'!$E$1:F68,2,FALSE)</f>
+        <f>VLOOKUP(F65,'Source lists'!$E$1:F67,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J65" s="1">
-        <f>VLOOKUP(G65,'Source lists'!$H$1:I69,2,FALSE)</f>
+        <f>VLOOKUP(G65,'Source lists'!$H$1:I68,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K65" s="1">
@@ -6059,18 +6055,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L65">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>167</v>
@@ -6085,11 +6081,11 @@
         <v>69</v>
       </c>
       <c r="I66" s="1">
-        <f>VLOOKUP(F66,'Source lists'!$E$1:F69,2,FALSE)</f>
+        <f>VLOOKUP(F66,'Source lists'!$E$1:F68,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J66" s="1">
-        <f>VLOOKUP(G66,'Source lists'!$H$1:I70,2,FALSE)</f>
+        <f>VLOOKUP(G66,'Source lists'!$H$1:I69,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K66" s="1">
@@ -6097,18 +6093,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L66">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>167</v>
@@ -6123,11 +6119,11 @@
         <v>69</v>
       </c>
       <c r="I67" s="1">
-        <f>VLOOKUP(F67,'Source lists'!$E$1:F70,2,FALSE)</f>
+        <f>VLOOKUP(F67,'Source lists'!$E$1:F69,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J67" s="1">
-        <f>VLOOKUP(G67,'Source lists'!$H$1:I71,2,FALSE)</f>
+        <f>VLOOKUP(G67,'Source lists'!$H$1:I70,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K67" s="1">
@@ -6135,18 +6131,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L67">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B68" t="s">
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>167</v>
@@ -6161,11 +6157,11 @@
         <v>69</v>
       </c>
       <c r="I68" s="1">
-        <f>VLOOKUP(F68,'Source lists'!$E$1:F71,2,FALSE)</f>
+        <f>VLOOKUP(F68,'Source lists'!$E$1:F70,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J68" s="1">
-        <f>VLOOKUP(G68,'Source lists'!$H$1:I72,2,FALSE)</f>
+        <f>VLOOKUP(G68,'Source lists'!$H$1:I71,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K68" s="1">
@@ -6173,18 +6169,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L68">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>167</v>
@@ -6199,11 +6195,11 @@
         <v>69</v>
       </c>
       <c r="I69" s="1">
-        <f>VLOOKUP(F69,'Source lists'!$E$1:F72,2,FALSE)</f>
+        <f>VLOOKUP(F69,'Source lists'!$E$1:F71,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J69" s="1">
-        <f>VLOOKUP(G69,'Source lists'!$H$1:I73,2,FALSE)</f>
+        <f>VLOOKUP(G69,'Source lists'!$H$1:I72,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K69" s="1">
@@ -6211,21 +6207,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L69">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="F70" t="s">
         <v>17</v>
@@ -6237,11 +6233,11 @@
         <v>69</v>
       </c>
       <c r="I70" s="1">
-        <f>VLOOKUP(F70,'Source lists'!$E$1:F73,2,FALSE)</f>
+        <f>VLOOKUP(F70,'Source lists'!$E$1:F72,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J70" s="1">
-        <f>VLOOKUP(G70,'Source lists'!$H$1:I74,2,FALSE)</f>
+        <f>VLOOKUP(G70,'Source lists'!$H$1:I73,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K70" s="1">
@@ -6249,12 +6245,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L70">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
@@ -6275,11 +6271,11 @@
         <v>69</v>
       </c>
       <c r="I71" s="1">
-        <f>VLOOKUP(F71,'Source lists'!$E$1:F74,2,FALSE)</f>
+        <f>VLOOKUP(F71,'Source lists'!$E$1:F73,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J71" s="1">
-        <f>VLOOKUP(G71,'Source lists'!$H$1:I75,2,FALSE)</f>
+        <f>VLOOKUP(G71,'Source lists'!$H$1:I74,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K71" s="1">
@@ -6287,21 +6283,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L71">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F72" t="s">
         <v>17</v>
@@ -6313,11 +6309,11 @@
         <v>69</v>
       </c>
       <c r="I72" s="1">
-        <f>VLOOKUP(F72,'Source lists'!$E$1:F75,2,FALSE)</f>
+        <f>VLOOKUP(F72,'Source lists'!$E$1:F74,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J72" s="1">
-        <f>VLOOKUP(G72,'Source lists'!$H$1:I76,2,FALSE)</f>
+        <f>VLOOKUP(G72,'Source lists'!$H$1:I75,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K72" s="1">
@@ -6325,12 +6321,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L72">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
@@ -6339,7 +6335,7 @@
         <v>169</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F73" t="s">
         <v>17</v>
@@ -6351,11 +6347,11 @@
         <v>69</v>
       </c>
       <c r="I73" s="1">
-        <f>VLOOKUP(F73,'Source lists'!$E$1:F76,2,FALSE)</f>
+        <f>VLOOKUP(F73,'Source lists'!$E$1:F75,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J73" s="1">
-        <f>VLOOKUP(G73,'Source lists'!$H$1:I77,2,FALSE)</f>
+        <f>VLOOKUP(G73,'Source lists'!$H$1:I76,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K73" s="1">
@@ -6363,21 +6359,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L73">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F74" t="s">
         <v>17</v>
@@ -6389,11 +6385,11 @@
         <v>69</v>
       </c>
       <c r="I74" s="1">
-        <f>VLOOKUP(F74,'Source lists'!$E$1:F77,2,FALSE)</f>
+        <f>VLOOKUP(F74,'Source lists'!$E$1:F76,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J74" s="1">
-        <f>VLOOKUP(G74,'Source lists'!$H$1:I78,2,FALSE)</f>
+        <f>VLOOKUP(G74,'Source lists'!$H$1:I77,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K74" s="1">
@@ -6401,12 +6397,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L74">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
@@ -6415,7 +6411,7 @@
         <v>170</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="F75" t="s">
         <v>17</v>
@@ -6427,11 +6423,11 @@
         <v>69</v>
       </c>
       <c r="I75" s="1">
-        <f>VLOOKUP(F75,'Source lists'!$E$1:F78,2,FALSE)</f>
+        <f>VLOOKUP(F75,'Source lists'!$E$1:F77,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J75" s="1">
-        <f>VLOOKUP(G75,'Source lists'!$H$1:I79,2,FALSE)</f>
+        <f>VLOOKUP(G75,'Source lists'!$H$1:I78,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K75" s="1">
@@ -6439,56 +6435,59 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L75">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>84</v>
+        <v>172</v>
       </c>
       <c r="F76" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G76" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H76" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="I76" s="1">
-        <f>VLOOKUP(F76,'Source lists'!$E$1:F79,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F76,'Source lists'!$E$1:F78,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J76" s="1">
-        <f>VLOOKUP(G76,'Source lists'!$H$1:I80,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G76,'Source lists'!$H$1:I79,2,FALSE)</f>
+        <v>10</v>
       </c>
       <c r="K76" s="1">
         <f>VLOOKUP(F76,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G76,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H76,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>14.285714285714286</v>
+      </c>
+      <c r="L76">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A77">
+        <v>35</v>
+      </c>
+      <c r="B77" t="s">
         <v>38</v>
       </c>
-      <c r="B77" t="s">
-        <v>1</v>
-      </c>
       <c r="C77" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F77" t="s">
         <v>16</v>
@@ -6500,11 +6499,11 @@
         <v>23</v>
       </c>
       <c r="I77" s="1">
-        <f>VLOOKUP(F77,'Source lists'!$E$1:F80,2,FALSE)</f>
+        <f>VLOOKUP(F77,'Source lists'!$E$1:F79,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J77" s="1">
-        <f>VLOOKUP(G77,'Source lists'!$H$1:I81,2,FALSE)</f>
+        <f>VLOOKUP(G77,'Source lists'!$H$1:I80,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K77" s="1">
@@ -6512,21 +6511,18 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B78" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>133</v>
-      </c>
-      <c r="D78" t="s">
-        <v>188</v>
+        <v>87</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
@@ -6538,11 +6534,11 @@
         <v>23</v>
       </c>
       <c r="I78" s="1">
-        <f>VLOOKUP(F78,'Source lists'!$E$1:F81,2,FALSE)</f>
+        <f>VLOOKUP(F78,'Source lists'!$E$1:F80,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J78" s="1">
-        <f>VLOOKUP(G78,'Source lists'!$H$1:I82,2,FALSE)</f>
+        <f>VLOOKUP(G78,'Source lists'!$H$1:I81,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K78" s="1">
@@ -6550,9 +6546,9 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
@@ -6564,7 +6560,7 @@
         <v>188</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="F79" t="s">
         <v>16</v>
@@ -6576,11 +6572,11 @@
         <v>23</v>
       </c>
       <c r="I79" s="1">
-        <f>VLOOKUP(F79,'Source lists'!$E$1:F82,2,FALSE)</f>
+        <f>VLOOKUP(F79,'Source lists'!$E$1:F81,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J79" s="1">
-        <f>VLOOKUP(G79,'Source lists'!$H$1:I83,2,FALSE)</f>
+        <f>VLOOKUP(G79,'Source lists'!$H$1:I82,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K79" s="1">
@@ -6588,18 +6584,21 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>150</v>
+        <v>133</v>
+      </c>
+      <c r="D80" t="s">
+        <v>188</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="F80" t="s">
         <v>16</v>
@@ -6611,11 +6610,11 @@
         <v>23</v>
       </c>
       <c r="I80" s="1">
-        <f>VLOOKUP(F80,'Source lists'!$E$1:F83,2,FALSE)</f>
+        <f>VLOOKUP(F80,'Source lists'!$E$1:F82,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J80" s="1">
-        <f>VLOOKUP(G80,'Source lists'!$H$1:I84,2,FALSE)</f>
+        <f>VLOOKUP(G80,'Source lists'!$H$1:I83,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K80" s="1">
@@ -6625,7 +6624,7 @@
     </row>
     <row r="81" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
@@ -6634,7 +6633,7 @@
         <v>150</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F81" t="s">
         <v>16</v>
@@ -6646,11 +6645,11 @@
         <v>23</v>
       </c>
       <c r="I81" s="1">
-        <f>VLOOKUP(F81,'Source lists'!$E$1:F84,2,FALSE)</f>
+        <f>VLOOKUP(F81,'Source lists'!$E$1:F83,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J81" s="1">
-        <f>VLOOKUP(G81,'Source lists'!$H$1:I85,2,FALSE)</f>
+        <f>VLOOKUP(G81,'Source lists'!$H$1:I84,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K81" s="1">
@@ -6660,51 +6659,48 @@
     </row>
     <row r="82" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>73</v>
-      </c>
-      <c r="D82" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="F82" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G82" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H82" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="I82" s="1">
-        <f>VLOOKUP(F82,'Source lists'!$E$1:F85,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F82,'Source lists'!$E$1:F84,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J82" s="1">
-        <f>VLOOKUP(G82,'Source lists'!$H$1:I86,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G82,'Source lists'!$H$1:I85,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K82" s="1">
         <f>VLOOKUP(F82,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G82,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H82,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.8</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B83" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C83" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -6722,11 +6718,11 @@
         <v>70</v>
       </c>
       <c r="I83" s="1">
-        <f>VLOOKUP(F83,'Source lists'!$E$1:F86,2,FALSE)</f>
+        <f>VLOOKUP(F83,'Source lists'!$E$1:F85,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J83" s="1">
-        <f>VLOOKUP(G83,'Source lists'!$H$1:I87,2,FALSE)</f>
+        <f>VLOOKUP(G83,'Source lists'!$H$1:I86,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K83" s="1">
@@ -6734,21 +6730,21 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B84" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D84" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="F84" t="s">
         <v>15</v>
@@ -6760,11 +6756,11 @@
         <v>70</v>
       </c>
       <c r="I84" s="1">
-        <f>VLOOKUP(F84,'Source lists'!$E$1:F87,2,FALSE)</f>
+        <f>VLOOKUP(F84,'Source lists'!$E$1:F86,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J84" s="1">
-        <f>VLOOKUP(G84,'Source lists'!$H$1:I88,2,FALSE)</f>
+        <f>VLOOKUP(G84,'Source lists'!$H$1:I87,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K84" s="1">
@@ -6772,9 +6768,9 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
@@ -6786,7 +6782,7 @@
         <v>112</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F85" t="s">
         <v>15</v>
@@ -6798,11 +6794,11 @@
         <v>70</v>
       </c>
       <c r="I85" s="1">
-        <f>VLOOKUP(F85,'Source lists'!$E$1:F88,2,FALSE)</f>
+        <f>VLOOKUP(F85,'Source lists'!$E$1:F87,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J85" s="1">
-        <f>VLOOKUP(G85,'Source lists'!$H$1:I89,2,FALSE)</f>
+        <f>VLOOKUP(G85,'Source lists'!$H$1:I88,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K85" s="1">
@@ -6810,9 +6806,9 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
@@ -6820,8 +6816,11 @@
       <c r="C86" t="s">
         <v>91</v>
       </c>
+      <c r="D86" t="s">
+        <v>112</v>
+      </c>
       <c r="E86" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F86" t="s">
         <v>15</v>
@@ -6833,11 +6832,11 @@
         <v>70</v>
       </c>
       <c r="I86" s="1">
-        <f>VLOOKUP(F86,'Source lists'!$E$1:F89,2,FALSE)</f>
+        <f>VLOOKUP(F86,'Source lists'!$E$1:F88,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J86" s="1">
-        <f>VLOOKUP(G86,'Source lists'!$H$1:I90,2,FALSE)</f>
+        <f>VLOOKUP(G86,'Source lists'!$H$1:I89,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K86" s="1">
@@ -6845,56 +6844,56 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>87</v>
-      </c>
-      <c r="D87" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F87" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G87" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H87" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="I87" s="1">
-        <f>VLOOKUP(F87,'Source lists'!$E$1:F90,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F87,'Source lists'!$E$1:F89,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J87" s="1">
-        <f>VLOOKUP(G87,'Source lists'!$H$1:I91,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(G87,'Source lists'!$H$1:I90,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K87" s="1">
         <f>VLOOKUP(F87,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G87,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H87,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B88" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>104</v>
+        <v>87</v>
+      </c>
+      <c r="D88" t="s">
+        <v>89</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="F88" t="s">
         <v>17</v>
@@ -6906,11 +6905,11 @@
         <v>22</v>
       </c>
       <c r="I88" s="1">
-        <f>VLOOKUP(F88,'Source lists'!$E$1:F91,2,FALSE)</f>
+        <f>VLOOKUP(F88,'Source lists'!$E$1:F90,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J88" s="1">
-        <f>VLOOKUP(G88,'Source lists'!$H$1:I92,2,FALSE)</f>
+        <f>VLOOKUP(G88,'Source lists'!$H$1:I91,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K88" s="1">
@@ -6918,18 +6917,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B89" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="F89" t="s">
         <v>17</v>
@@ -6941,11 +6940,11 @@
         <v>22</v>
       </c>
       <c r="I89" s="1">
-        <f>VLOOKUP(F89,'Source lists'!$E$1:F92,2,FALSE)</f>
+        <f>VLOOKUP(F89,'Source lists'!$E$1:F91,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J89" s="1">
-        <f>VLOOKUP(G89,'Source lists'!$H$1:I93,2,FALSE)</f>
+        <f>VLOOKUP(G89,'Source lists'!$H$1:I92,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K89" s="1">
@@ -6953,18 +6952,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="F90" t="s">
         <v>17</v>
@@ -6976,11 +6975,11 @@
         <v>22</v>
       </c>
       <c r="I90" s="1">
-        <f>VLOOKUP(F90,'Source lists'!$E$1:F93,2,FALSE)</f>
+        <f>VLOOKUP(F90,'Source lists'!$E$1:F92,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J90" s="1">
-        <f>VLOOKUP(G90,'Source lists'!$H$1:I94,2,FALSE)</f>
+        <f>VLOOKUP(G90,'Source lists'!$H$1:I93,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K90" s="1">
@@ -6988,18 +6987,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="F91" t="s">
         <v>17</v>
@@ -7011,11 +7010,11 @@
         <v>22</v>
       </c>
       <c r="I91" s="1">
-        <f>VLOOKUP(F91,'Source lists'!$E$1:F94,2,FALSE)</f>
+        <f>VLOOKUP(F91,'Source lists'!$E$1:F93,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J91" s="1">
-        <f>VLOOKUP(G91,'Source lists'!$H$1:I95,2,FALSE)</f>
+        <f>VLOOKUP(G91,'Source lists'!$H$1:I94,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K91" s="1">
@@ -7023,18 +7022,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="F92" t="s">
         <v>17</v>
@@ -7046,11 +7045,11 @@
         <v>22</v>
       </c>
       <c r="I92" s="1">
-        <f>VLOOKUP(F92,'Source lists'!$E$1:F95,2,FALSE)</f>
+        <f>VLOOKUP(F92,'Source lists'!$E$1:F94,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J92" s="1">
-        <f>VLOOKUP(G92,'Source lists'!$H$1:I96,2,FALSE)</f>
+        <f>VLOOKUP(G92,'Source lists'!$H$1:I95,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K92" s="1">
@@ -7058,18 +7057,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="B93" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>117</v>
+        <v>196</v>
       </c>
       <c r="F93" t="s">
         <v>17</v>
@@ -7078,30 +7077,33 @@
         <v>26</v>
       </c>
       <c r="H93" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I93" s="1">
-        <f>VLOOKUP(F93,'Source lists'!$E$1:F96,2,FALSE)</f>
+        <f>VLOOKUP(F93,'Source lists'!$E$1:F95,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J93" s="1">
-        <f>VLOOKUP(G93,'Source lists'!$H$1:I97,2,FALSE)</f>
+        <f>VLOOKUP(G93,'Source lists'!$H$1:I96,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K93" s="1">
         <f>VLOOKUP(F93,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G93,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H93,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B94" t="s">
-        <v>7</v>
+        <v>66</v>
+      </c>
+      <c r="C94" t="s">
+        <v>82</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F94" t="s">
         <v>17</v>
@@ -7113,11 +7115,11 @@
         <v>21</v>
       </c>
       <c r="I94" s="1">
-        <f>VLOOKUP(F94,'Source lists'!$E$1:F97,2,FALSE)</f>
+        <f>VLOOKUP(F94,'Source lists'!$E$1:F96,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J94" s="1">
-        <f>VLOOKUP(G94,'Source lists'!$H$1:I98,2,FALSE)</f>
+        <f>VLOOKUP(G94,'Source lists'!$H$1:I97,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K94" s="1">
@@ -7125,15 +7127,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B95" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F95" t="s">
         <v>17</v>
@@ -7145,11 +7147,11 @@
         <v>21</v>
       </c>
       <c r="I95" s="1">
-        <f>VLOOKUP(F95,'Source lists'!$E$1:F98,2,FALSE)</f>
+        <f>VLOOKUP(F95,'Source lists'!$E$1:F97,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J95" s="1">
-        <f>VLOOKUP(G95,'Source lists'!$H$1:I99,2,FALSE)</f>
+        <f>VLOOKUP(G95,'Source lists'!$H$1:I98,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K95" s="1">
@@ -7157,18 +7159,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="F96" t="s">
         <v>17</v>
@@ -7180,11 +7179,11 @@
         <v>21</v>
       </c>
       <c r="I96" s="1">
-        <f>VLOOKUP(F96,'Source lists'!$E$1:F99,2,FALSE)</f>
+        <f>VLOOKUP(F96,'Source lists'!$E$1:F98,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J96" s="1">
-        <f>VLOOKUP(G96,'Source lists'!$H$1:I100,2,FALSE)</f>
+        <f>VLOOKUP(G96,'Source lists'!$H$1:I99,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K96" s="1">
@@ -7192,18 +7191,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B97" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F97" t="s">
         <v>17</v>
@@ -7215,11 +7214,11 @@
         <v>21</v>
       </c>
       <c r="I97" s="1">
-        <f>VLOOKUP(F97,'Source lists'!$E$1:F100,2,FALSE)</f>
+        <f>VLOOKUP(F97,'Source lists'!$E$1:F99,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J97" s="1">
-        <f>VLOOKUP(G97,'Source lists'!$H$1:I101,2,FALSE)</f>
+        <f>VLOOKUP(G97,'Source lists'!$H$1:I100,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K97" s="1">
@@ -7227,53 +7226,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A98">
+        <v>99</v>
+      </c>
+      <c r="B98" t="s">
+        <v>168</v>
+      </c>
+      <c r="C98" t="s">
+        <v>169</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F98" t="s">
+        <v>17</v>
+      </c>
+      <c r="G98" t="s">
         <v>26</v>
       </c>
-      <c r="B98" t="s">
-        <v>66</v>
-      </c>
-      <c r="C98" t="s">
-        <v>73</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F98" t="s">
-        <v>16</v>
-      </c>
-      <c r="G98" t="s">
-        <v>29</v>
-      </c>
       <c r="H98" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I98" s="1">
-        <f>VLOOKUP(F98,'Source lists'!$E$1:F101,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F98,'Source lists'!$E$1:F100,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J98" s="1">
-        <f>VLOOKUP(G98,'Source lists'!$H$1:I102,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G98,'Source lists'!$H$1:I101,2,FALSE)</f>
+        <v>10</v>
       </c>
       <c r="K98" s="1">
         <f>VLOOKUP(F98,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G98,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H98,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B99" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C99" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="F99" t="s">
         <v>16</v>
@@ -7285,11 +7284,11 @@
         <v>24</v>
       </c>
       <c r="I99" s="1">
-        <f>VLOOKUP(F99,'Source lists'!$E$1:F102,2,FALSE)</f>
+        <f>VLOOKUP(F99,'Source lists'!$E$1:F101,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J99" s="1">
-        <f>VLOOKUP(G99,'Source lists'!$H$1:I103,2,FALSE)</f>
+        <f>VLOOKUP(G99,'Source lists'!$H$1:I102,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K99" s="1">
@@ -7297,18 +7296,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B100" t="s">
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="F100" t="s">
         <v>16</v>
@@ -7320,11 +7319,11 @@
         <v>24</v>
       </c>
       <c r="I100" s="1">
-        <f>VLOOKUP(F100,'Source lists'!$E$1:F103,2,FALSE)</f>
+        <f>VLOOKUP(F100,'Source lists'!$E$1:F102,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J100" s="1">
-        <f>VLOOKUP(G100,'Source lists'!$H$1:I104,2,FALSE)</f>
+        <f>VLOOKUP(G100,'Source lists'!$H$1:I103,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K100" s="1">
@@ -7334,7 +7333,7 @@
     </row>
     <row r="101" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
@@ -7343,7 +7342,7 @@
         <v>91</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F101" t="s">
         <v>16</v>
@@ -7355,11 +7354,11 @@
         <v>24</v>
       </c>
       <c r="I101" s="1">
-        <f>VLOOKUP(F101,'Source lists'!$E$1:F104,2,FALSE)</f>
+        <f>VLOOKUP(F101,'Source lists'!$E$1:F103,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J101" s="1">
-        <f>VLOOKUP(G101,'Source lists'!$H$1:I105,2,FALSE)</f>
+        <f>VLOOKUP(G101,'Source lists'!$H$1:I104,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K101" s="1">
@@ -7367,35 +7366,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>199</v>
+        <v>98</v>
       </c>
       <c r="F102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G102" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="H102" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="I102" s="1">
-        <f>VLOOKUP(F102,'Source lists'!$E$1:F105,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F102,'Source lists'!$E$1:F104,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J102" s="1">
-        <f>VLOOKUP(G102,'Source lists'!$H$1:I106,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G102,'Source lists'!$H$1:I105,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K102" s="1">
         <f>VLOOKUP(F102,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G102,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H102,'Source lists'!$K$2:$L$9,2,FALSE)</f>
@@ -7404,7 +7403,7 @@
     </row>
     <row r="103" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B103" t="s">
         <v>2</v>
@@ -7413,7 +7412,7 @@
         <v>131</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F103" t="s">
         <v>17</v>
@@ -7425,11 +7424,11 @@
         <v>67</v>
       </c>
       <c r="I103" s="1">
-        <f>VLOOKUP(F103,'Source lists'!$E$1:F106,2,FALSE)</f>
+        <f>VLOOKUP(F103,'Source lists'!$E$1:F105,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J103" s="1">
-        <f>VLOOKUP(G103,'Source lists'!$H$1:I107,2,FALSE)</f>
+        <f>VLOOKUP(G103,'Source lists'!$H$1:I106,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K103" s="1">
@@ -7437,9 +7436,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B104" t="s">
         <v>2</v>
@@ -7448,7 +7447,7 @@
         <v>131</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="F104" t="s">
         <v>17</v>
@@ -7460,11 +7459,11 @@
         <v>67</v>
       </c>
       <c r="I104" s="1">
-        <f>VLOOKUP(F104,'Source lists'!$E$1:F107,2,FALSE)</f>
+        <f>VLOOKUP(F104,'Source lists'!$E$1:F106,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J104" s="1">
-        <f>VLOOKUP(G104,'Source lists'!$H$1:I108,2,FALSE)</f>
+        <f>VLOOKUP(G104,'Source lists'!$H$1:I107,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K104" s="1">
@@ -7474,19 +7473,16 @@
     </row>
     <row r="105" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B105" t="s">
         <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>133</v>
-      </c>
-      <c r="D105" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>201</v>
+        <v>132</v>
       </c>
       <c r="F105" t="s">
         <v>17</v>
@@ -7498,11 +7494,11 @@
         <v>67</v>
       </c>
       <c r="I105" s="1">
-        <f>VLOOKUP(F105,'Source lists'!$E$1:F108,2,FALSE)</f>
+        <f>VLOOKUP(F105,'Source lists'!$E$1:F107,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J105" s="1">
-        <f>VLOOKUP(G105,'Source lists'!$H$1:I109,2,FALSE)</f>
+        <f>VLOOKUP(G105,'Source lists'!$H$1:I108,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K105" s="1">
@@ -7510,18 +7506,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B106" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C106" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="D106" t="s">
+        <v>138</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="F106" t="s">
         <v>17</v>
@@ -7533,11 +7532,11 @@
         <v>67</v>
       </c>
       <c r="I106" s="1">
-        <f>VLOOKUP(F106,'Source lists'!$E$1:F109,2,FALSE)</f>
+        <f>VLOOKUP(F106,'Source lists'!$E$1:F108,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J106" s="1">
-        <f>VLOOKUP(G106,'Source lists'!$H$1:I110,2,FALSE)</f>
+        <f>VLOOKUP(G106,'Source lists'!$H$1:I109,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K106" s="1">
@@ -7547,156 +7546,156 @@
     </row>
     <row r="107" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="B107" t="s">
-        <v>75</v>
+        <v>3</v>
+      </c>
+      <c r="C107" t="s">
+        <v>142</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="F107" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G107" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="H107" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="I107" s="1">
-        <f>VLOOKUP(F107,'Source lists'!$E$1:F45,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F107,'Source lists'!$E$1:F109,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J107" s="1">
-        <f>VLOOKUP(G107,'Source lists'!$H$1:I46,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G107,'Source lists'!$H$1:I110,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K107" s="1">
         <f>VLOOKUP(F107,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G107,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H107,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="B108" t="s">
         <v>75</v>
       </c>
-      <c r="C108" t="s">
-        <v>102</v>
-      </c>
       <c r="E108" s="2" t="s">
-        <v>103</v>
+        <v>185</v>
       </c>
       <c r="F108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G108" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H108" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="I108" s="1">
-        <f>VLOOKUP(F108,'Source lists'!$E$1:F110,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F108,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J108" s="1">
-        <f>VLOOKUP(G108,'Source lists'!$H$1:I111,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(G108,'Source lists'!$H$1:I46,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K108" s="1">
         <f>VLOOKUP(F108,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G108,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H108,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>51</v>
+      </c>
+      <c r="B109" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" t="s">
+        <v>102</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F109" t="s">
+        <v>17</v>
+      </c>
+      <c r="G109" t="s">
+        <v>27</v>
+      </c>
+      <c r="H109" t="s">
+        <v>69</v>
+      </c>
+      <c r="I109" s="1">
+        <f>VLOOKUP(F109,'Source lists'!$E$1:F110,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J109" s="1">
+        <f>VLOOKUP(G109,'Source lists'!$H$1:I111,2,FALSE)</f>
         <v>7</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109">
-        <v>28</v>
-      </c>
-      <c r="B109" t="s">
-        <v>66</v>
-      </c>
-      <c r="C109" t="s">
-        <v>73</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F109" t="s">
-        <v>16</v>
-      </c>
-      <c r="G109" t="s">
-        <v>29</v>
-      </c>
-      <c r="H109" t="s">
-        <v>67</v>
-      </c>
-      <c r="I109" s="1">
-        <f>VLOOKUP(F109,'Source lists'!$E$1:F111,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="J109" s="1">
-        <f>VLOOKUP(G109,'Source lists'!$H$1:I112,2,FALSE)</f>
-        <v>3</v>
       </c>
       <c r="K109" s="1">
         <f>VLOOKUP(F109,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G109,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H109,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="B110" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C110" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="F110" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G110" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H110" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="I110" s="1">
-        <f>VLOOKUP(F110,'Source lists'!$E$1:F46,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F110,'Source lists'!$E$1:F111,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J110" s="1">
-        <f>VLOOKUP(G110,'Source lists'!$H$1:I47,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(G110,'Source lists'!$H$1:I112,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K110" s="1">
         <f>VLOOKUP(F110,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G110,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H110,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>111</v>
+      </c>
+      <c r="B111" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111">
-        <v>29</v>
-      </c>
-      <c r="B111" t="s">
-        <v>66</v>
-      </c>
       <c r="C111" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="F111" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G111" t="s">
         <v>30</v>
@@ -7705,27 +7704,27 @@
         <v>23</v>
       </c>
       <c r="I111" s="1">
-        <f>VLOOKUP(F111,'Source lists'!$E$1:F112,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F111,'Source lists'!$E$1:F46,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J111" s="1">
-        <f>VLOOKUP(G111,'Source lists'!$H$1:I113,2,FALSE)</f>
+        <f>VLOOKUP(G111,'Source lists'!$H$1:I47,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K111" s="1">
         <f>VLOOKUP(F111,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G111,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H111,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>1.5</v>
-      </c>
-      <c r="L111">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B112" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="C112" t="s">
+        <v>73</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>79</v>
@@ -7740,11 +7739,11 @@
         <v>23</v>
       </c>
       <c r="I112" s="1">
-        <f>VLOOKUP(F112,'Source lists'!$E$1:F113,2,FALSE)</f>
+        <f>VLOOKUP(F112,'Source lists'!$E$1:F112,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J112" s="1">
-        <f>VLOOKUP(G112,'Source lists'!$H$1:I114,2,FALSE)</f>
+        <f>VLOOKUP(G112,'Source lists'!$H$1:I113,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K112" s="1">
@@ -7755,18 +7754,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B113" t="s">
-        <v>75</v>
-      </c>
-      <c r="C113" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F113" t="s">
         <v>16</v>
@@ -7775,25 +7771,63 @@
         <v>30</v>
       </c>
       <c r="H113" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="I113" s="1">
-        <f>VLOOKUP(F113,'Source lists'!$E$1:F114,2,FALSE)</f>
+        <f>VLOOKUP(F113,'Source lists'!$E$1:F113,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J113" s="1">
-        <f>VLOOKUP(G113,'Source lists'!$H$1:I115,2,FALSE)</f>
+        <f>VLOOKUP(G113,'Source lists'!$H$1:I114,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K113" s="1">
         <f>VLOOKUP(F113,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G113,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H113,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="L113">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>27</v>
+      </c>
+      <c r="B114" t="s">
+        <v>75</v>
+      </c>
+      <c r="C114" t="s">
+        <v>76</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F114" t="s">
+        <v>16</v>
+      </c>
+      <c r="G114" t="s">
+        <v>30</v>
+      </c>
+      <c r="H114" t="s">
+        <v>69</v>
+      </c>
+      <c r="I114" s="1">
+        <f>VLOOKUP(F114,'Source lists'!$E$1:F114,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="J114" s="1">
+        <f>VLOOKUP(G114,'Source lists'!$H$1:I115,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K114" s="1">
+        <f>VLOOKUP(F114,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G114,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H114,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>0.42857142857142855</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M113">
-      <sortCondition descending="1" ref="K1:K113"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M114">
+      <sortCondition descending="1" ref="K1:K114"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7822,7 +7856,7 @@
           <x14:formula1>
             <xm:f>'Source lists'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB14BE7A-53BF-A94F-B394-C5FBF576D0FC}">
           <x14:formula1>

</xml_diff>

<commit_message>
e-Questrian/statements: Statements now correctly reflect credit notes where applicable
</commit_message>
<xml_diff>
--- a/e-Question - To do list.xlsx
+++ b/e-Question - To do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8365D22-B27C-3645-9544-DF730721D39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25BFD44-393C-FA46-A2C1-66E223562EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of completion" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="13" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="211">
   <si>
     <t>Sections</t>
   </si>
@@ -708,6 +708,9 @@
   </si>
   <si>
     <t>Needs to be a modal specfically for modals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment are not being recorded correctly </t>
   </si>
 </sst>
 </file>
@@ -797,13 +800,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45307.43574976852" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="114" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45307.534193402775" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="116" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:M1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
   <cacheFields count="13">
     <cacheField name="#" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="113"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="114"/>
     </cacheField>
     <cacheField name="Section" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -854,7 +857,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="114">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="116">
   <r>
     <n v="53"/>
     <s v="Calendar/Appointments"/>
@@ -928,6 +931,21 @@
     <n v="6"/>
     <n v="96"/>
     <n v="53"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="114"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="Payment are not being recorded correctly "/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Investigation and change"/>
+    <n v="8"/>
+    <n v="6"/>
+    <n v="96"/>
+    <m/>
     <x v="1"/>
   </r>
   <r>
@@ -1096,21 +1114,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="17"/>
-    <s v="Marketing"/>
-    <s v="Landing Page"/>
-    <s v="What's New Section"/>
-    <s v="Should be added to Landing page"/>
-    <s v="Poor UX"/>
-    <s v="New feature"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="7"/>
-    <n v="39.200000000000003"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
     <n v="4"/>
     <s v="Marketing"/>
     <s v="Landing Page"/>
@@ -1130,6 +1133,21 @@
     <s v="Marketing"/>
     <s v="Landing Page"/>
     <s v="Footer bar"/>
+    <s v="Should be added to Landing page"/>
+    <s v="Poor UX"/>
+    <s v="New feature"/>
+    <s v="New component/service with simple integration"/>
+    <n v="4"/>
+    <n v="7"/>
+    <n v="39.200000000000003"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <s v="Marketing"/>
+    <s v="Landing Page"/>
+    <s v="What's New Section"/>
     <s v="Should be added to Landing page"/>
     <s v="Poor UX"/>
     <s v="New feature"/>
@@ -2565,11 +2583,82 @@
     <m/>
     <x v="1"/>
   </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="12"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Priority S" fld="10" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:D15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2624,8 +2713,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2667,62 +2756,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Importance S" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colFields count="1">
-    <field x="12"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Priority S" fld="10" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3035,15 +3068,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CCC35A-14FA-1E40-8319-0349AC17C33D}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" max="3" activeRow="1" activeCol="1" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="12" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3067,19 +3110,19 @@
         <v>206</v>
       </c>
       <c r="B3" s="8">
-        <v>749</v>
+        <v>845</v>
       </c>
       <c r="C3" s="8">
         <v>2278.5976190476185</v>
       </c>
       <c r="D3" s="8">
-        <v>3027.5976190476185</v>
+        <v>3123.5976190476185</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="7">
         <f>GETPIVOTDATA("Priority S",$A$1,"Status","Done")/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.24739086703193092</v>
+        <v>0.27052139969860767</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3103,19 +3146,19 @@
         <v>183</v>
       </c>
       <c r="B9" s="8">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C9" s="8">
         <v>299</v>
       </c>
       <c r="D9" s="8">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="7">
         <f>GETPIVOTDATA("Importance S",$A$7,"Status","Done")/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.1601123595505618</v>
+        <v>0.17857142857142858</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3139,19 +3182,19 @@
         <v>184</v>
       </c>
       <c r="B15" s="8">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C15" s="8">
         <v>607</v>
       </c>
       <c r="D15" s="8">
-        <v>657</v>
+        <v>663</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="7">
         <f>GETPIVOTDATA("Impact S",$A$13,"Status","Done")/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>7.6103500761035003E-2</v>
+        <v>8.4464555052790352E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3580,10 +3623,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
-  <dimension ref="A1:M114"/>
+  <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3809,121 +3852,122 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>112</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D6"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="5">
         <f>VLOOKUP(F6,'Source lists'!$E$1:F117,2,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="5">
         <f>VLOOKUP(G6,'Source lists'!$H$1:I118,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="5">
         <f>VLOOKUP(F6,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G6,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H6,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>96</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <v>53</v>
       </c>
-      <c r="M6"/>
+      <c r="M6" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>45</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="A7">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
         <v>159</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="5">
-        <f>VLOOKUP(F7,'Source lists'!$E$1:F10,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="J7" s="5">
-        <f>VLOOKUP(G7,'Source lists'!$H$1:I11,2,FALSE)</f>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1">
+        <f>VLOOKUP(F7,'Source lists'!$E$1:F119,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="J7" s="1">
+        <f>VLOOKUP(G7,'Source lists'!$H$1:I120,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="1">
         <f>VLOOKUP(F7,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G7,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H7,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>72</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>176</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7"/>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E8" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>28</v>
+        <v>159</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I8" s="5">
-        <f>VLOOKUP(F8,'Source lists'!$E$1:F11,2,FALSE)</f>
+        <f>VLOOKUP(F8,'Source lists'!$E$1:F10,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J8" s="5">
-        <f>VLOOKUP(G8,'Source lists'!$H$1:I12,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G8,'Source lists'!$H$1:I11,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K8" s="5">
         <f>VLOOKUP(F8,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G8,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H8,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
@@ -3931,130 +3975,132 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="3">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="5">
+        <f>VLOOKUP(F9,'Source lists'!$E$1:F11,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="J9" s="5">
+        <f>VLOOKUP(G9,'Source lists'!$H$1:I12,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="K9" s="5">
+        <f>VLOOKUP(F9,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G9,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H9,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>113</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>207</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>208</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>159</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="1">
-        <f>VLOOKUP(F9,'Source lists'!$E$1:F118,2,FALSE)</f>
+      <c r="I10" s="1">
+        <f>VLOOKUP(F10,'Source lists'!$E$1:F118,2,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="J9" s="1">
-        <f>VLOOKUP(G9,'Source lists'!$H$1:I119,2,FALSE)</f>
+      <c r="J10" s="1">
+        <f>VLOOKUP(G10,'Source lists'!$H$1:I119,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="K9" s="1">
-        <f>VLOOKUP(F9,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G9,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H9,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+      <c r="K10" s="1">
+        <f>VLOOKUP(F10,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G10,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H10,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>57.6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="5">
-        <f>VLOOKUP(F10,'Source lists'!$E$1:F12,2,FALSE)</f>
+      <c r="I11" s="5">
+        <f>VLOOKUP(F11,'Source lists'!$E$1:F12,2,FALSE)</f>
         <v>10</v>
       </c>
-      <c r="J10" s="5">
-        <f>VLOOKUP(G10,'Source lists'!$H$1:I13,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="K10" s="5">
-        <f>VLOOKUP(F10,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G10,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H10,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+      <c r="J11" s="5">
+        <f>VLOOKUP(G11,'Source lists'!$H$1:I13,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="K11" s="5">
+        <f>VLOOKUP(F11,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G11,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H11,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>53.333333333333336</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3" t="s">
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>59</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="1">
-        <f>VLOOKUP(F11,'Source lists'!$E$1:F13,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
-        <f>VLOOKUP(G11,'Source lists'!$H$1:I14,2,FALSE)</f>
-        <v>10</v>
-      </c>
-      <c r="K11" s="1">
-        <f>VLOOKUP(F11,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G11,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H11,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>50</v>
-      </c>
-      <c r="L11">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -4066,11 +4112,11 @@
         <v>23</v>
       </c>
       <c r="I12" s="1">
-        <f>VLOOKUP(F12,'Source lists'!$E$1:F14,2,FALSE)</f>
+        <f>VLOOKUP(F12,'Source lists'!$E$1:F13,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J12" s="1">
-        <f>VLOOKUP(G12,'Source lists'!$H$1:I15,2,FALSE)</f>
+        <f>VLOOKUP(G12,'Source lists'!$H$1:I14,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K12" s="1">
@@ -4078,12 +4124,12 @@
         <v>50</v>
       </c>
       <c r="L12">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -4093,7 +4139,7 @@
       </c>
       <c r="D13"/>
       <c r="E13" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -4105,11 +4151,11 @@
         <v>23</v>
       </c>
       <c r="I13" s="1">
-        <f>VLOOKUP(F13,'Source lists'!$E$1:F15,2,FALSE)</f>
+        <f>VLOOKUP(F13,'Source lists'!$E$1:F14,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J13" s="1">
-        <f>VLOOKUP(G13,'Source lists'!$H$1:I16,2,FALSE)</f>
+        <f>VLOOKUP(G13,'Source lists'!$H$1:I15,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K13" s="1">
@@ -4117,22 +4163,22 @@
         <v>50</v>
       </c>
       <c r="L13">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M13"/>
     </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -4144,11 +4190,11 @@
         <v>23</v>
       </c>
       <c r="I14" s="1">
-        <f>VLOOKUP(F14,'Source lists'!$E$1:F16,2,FALSE)</f>
+        <f>VLOOKUP(F14,'Source lists'!$E$1:F15,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J14" s="1">
-        <f>VLOOKUP(G14,'Source lists'!$H$1:I17,2,FALSE)</f>
+        <f>VLOOKUP(G14,'Source lists'!$H$1:I16,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K14" s="1">
@@ -4156,90 +4202,90 @@
         <v>50</v>
       </c>
       <c r="L14">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="1">
+        <f>VLOOKUP(F15,'Source lists'!$E$1:F16,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <f>VLOOKUP(G15,'Source lists'!$H$1:I17,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="K15" s="1">
+        <f>VLOOKUP(F15,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G15,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H15,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="L15">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
         <v>40</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="5">
-        <f>VLOOKUP(F15,'Source lists'!$E$1:F17,2,FALSE)</f>
+      <c r="I16" s="5">
+        <f>VLOOKUP(F16,'Source lists'!$E$1:F17,2,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="J15" s="5">
-        <f>VLOOKUP(G15,'Source lists'!$H$1:I18,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="K15" s="5">
-        <f>VLOOKUP(F15,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G15,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H15,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+      <c r="J16" s="5">
+        <f>VLOOKUP(G16,'Source lists'!$H$1:I18,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="K16" s="5">
+        <f>VLOOKUP(F16,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G16,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H16,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>42.666666666666664</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3" t="s">
+      <c r="L16" s="3"/>
+      <c r="M16" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="17" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" s="1">
-        <f>VLOOKUP(F16,'Source lists'!$E$1:F18,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="J16" s="1">
-        <f>VLOOKUP(G16,'Source lists'!$H$1:I19,2,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="K16" s="1">
-        <f>VLOOKUP(F16,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G16,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H16,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>39.200000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
@@ -4248,10 +4294,10 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -4263,11 +4309,11 @@
         <v>70</v>
       </c>
       <c r="I17" s="1">
-        <f>VLOOKUP(F17,'Source lists'!$E$1:F19,2,FALSE)</f>
+        <f>VLOOKUP(F17,'Source lists'!$E$1:F18,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J17" s="1">
-        <f>VLOOKUP(G17,'Source lists'!$H$1:I20,2,FALSE)</f>
+        <f>VLOOKUP(G17,'Source lists'!$H$1:I19,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K17" s="1">
@@ -4277,8 +4323,7 @@
     </row>
     <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>A57</f>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -4287,7 +4332,7 @@
         <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>95</v>
@@ -4302,11 +4347,11 @@
         <v>70</v>
       </c>
       <c r="I18" s="1">
-        <f>VLOOKUP(F18,'Source lists'!$E$1:F20,2,FALSE)</f>
+        <f>VLOOKUP(F18,'Source lists'!$E$1:F19,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J18" s="1">
-        <f>VLOOKUP(G18,'Source lists'!$H$1:I21,2,FALSE)</f>
+        <f>VLOOKUP(G18,'Source lists'!$H$1:I20,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K18" s="1">
@@ -4390,21 +4435,22 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>24</v>
+        <f>A60</f>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
@@ -4416,11 +4462,11 @@
         <v>70</v>
       </c>
       <c r="I21" s="1">
-        <f>VLOOKUP(F21,'Source lists'!$E$1:F23,2,FALSE)</f>
+        <f>VLOOKUP(F21,'Source lists'!$E$1:F20,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J21" s="1">
-        <f>VLOOKUP(G21,'Source lists'!$H$1:I24,2,FALSE)</f>
+        <f>VLOOKUP(G21,'Source lists'!$H$1:I21,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K21" s="1">
@@ -4428,9 +4474,9 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -4438,34 +4484,37 @@
       <c r="C22" t="s">
         <v>42</v>
       </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
       <c r="E22" s="2" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I22" s="1">
-        <f>VLOOKUP(F22,'Source lists'!$E$1:F24,2,FALSE)</f>
+        <f>VLOOKUP(F22,'Source lists'!$E$1:F23,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J22" s="1">
-        <f>VLOOKUP(G22,'Source lists'!$H$1:I25,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G22,'Source lists'!$H$1:I24,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K22" s="1">
         <f>VLOOKUP(F22,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G22,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H22,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -4473,11 +4522,8 @@
       <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="D23" t="s">
-        <v>44</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
@@ -4489,24 +4535,21 @@
         <v>23</v>
       </c>
       <c r="I23" s="1">
-        <f>VLOOKUP(F23,'Source lists'!$E$1:F25,2,FALSE)</f>
+        <f>VLOOKUP(F23,'Source lists'!$E$1:F24,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J23" s="1">
-        <f>VLOOKUP(G23,'Source lists'!$H$1:I26,2,FALSE)</f>
+        <f>VLOOKUP(G23,'Source lists'!$H$1:I25,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K23" s="1">
         <f>VLOOKUP(F23,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G23,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H23,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L23">
-        <v>8</v>
-      </c>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -4518,7 +4561,7 @@
         <v>44</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
@@ -4530,11 +4573,11 @@
         <v>23</v>
       </c>
       <c r="I24" s="1">
-        <f>VLOOKUP(F24,'Source lists'!$E$1:F26,2,FALSE)</f>
+        <f>VLOOKUP(F24,'Source lists'!$E$1:F25,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J24" s="1">
-        <f>VLOOKUP(G24,'Source lists'!$H$1:I27,2,FALSE)</f>
+        <f>VLOOKUP(G24,'Source lists'!$H$1:I26,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K24" s="1">
@@ -4547,7 +4590,7 @@
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -4559,7 +4602,7 @@
         <v>44</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
@@ -4571,11 +4614,11 @@
         <v>23</v>
       </c>
       <c r="I25" s="1">
-        <f>VLOOKUP(F25,'Source lists'!$E$1:F27,2,FALSE)</f>
+        <f>VLOOKUP(F25,'Source lists'!$E$1:F26,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J25" s="1">
-        <f>VLOOKUP(G25,'Source lists'!$H$1:I28,2,FALSE)</f>
+        <f>VLOOKUP(G25,'Source lists'!$H$1:I27,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K25" s="1">
@@ -4588,7 +4631,7 @@
     </row>
     <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -4600,7 +4643,7 @@
         <v>44</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -4612,11 +4655,11 @@
         <v>23</v>
       </c>
       <c r="I26" s="1">
-        <f>VLOOKUP(F26,'Source lists'!$E$1:F28,2,FALSE)</f>
+        <f>VLOOKUP(F26,'Source lists'!$E$1:F27,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J26" s="1">
-        <f>VLOOKUP(G26,'Source lists'!$H$1:I29,2,FALSE)</f>
+        <f>VLOOKUP(G26,'Source lists'!$H$1:I28,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K26" s="1">
@@ -4629,7 +4672,7 @@
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -4641,7 +4684,7 @@
         <v>44</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -4653,11 +4696,11 @@
         <v>23</v>
       </c>
       <c r="I27" s="1">
-        <f>VLOOKUP(F27,'Source lists'!$E$1:F29,2,FALSE)</f>
+        <f>VLOOKUP(F27,'Source lists'!$E$1:F28,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J27" s="1">
-        <f>VLOOKUP(G27,'Source lists'!$H$1:I30,2,FALSE)</f>
+        <f>VLOOKUP(G27,'Source lists'!$H$1:I29,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K27" s="1">
@@ -4670,7 +4713,7 @@
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -4682,7 +4725,7 @@
         <v>44</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
@@ -4694,11 +4737,11 @@
         <v>23</v>
       </c>
       <c r="I28" s="1">
-        <f>VLOOKUP(F28,'Source lists'!$E$1:F30,2,FALSE)</f>
+        <f>VLOOKUP(F28,'Source lists'!$E$1:F29,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J28" s="1">
-        <f>VLOOKUP(G28,'Source lists'!$H$1:I31,2,FALSE)</f>
+        <f>VLOOKUP(G28,'Source lists'!$H$1:I30,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K28" s="1">
@@ -4711,7 +4754,7 @@
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -4723,7 +4766,7 @@
         <v>44</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
@@ -4735,11 +4778,11 @@
         <v>23</v>
       </c>
       <c r="I29" s="1">
-        <f>VLOOKUP(F29,'Source lists'!$E$1:F31,2,FALSE)</f>
+        <f>VLOOKUP(F29,'Source lists'!$E$1:F30,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J29" s="1">
-        <f>VLOOKUP(G29,'Source lists'!$H$1:I32,2,FALSE)</f>
+        <f>VLOOKUP(G29,'Source lists'!$H$1:I31,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K29" s="1">
@@ -4752,7 +4795,7 @@
     </row>
     <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -4764,7 +4807,7 @@
         <v>44</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -4776,11 +4819,11 @@
         <v>23</v>
       </c>
       <c r="I30" s="1">
-        <f>VLOOKUP(F30,'Source lists'!$E$1:F32,2,FALSE)</f>
+        <f>VLOOKUP(F30,'Source lists'!$E$1:F31,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J30" s="1">
-        <f>VLOOKUP(G30,'Source lists'!$H$1:I33,2,FALSE)</f>
+        <f>VLOOKUP(G30,'Source lists'!$H$1:I32,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K30" s="1">
@@ -4793,7 +4836,7 @@
     </row>
     <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -4802,10 +4845,10 @@
         <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F31" t="s">
         <v>15</v>
@@ -4817,30 +4860,36 @@
         <v>23</v>
       </c>
       <c r="I31" s="1">
-        <f>VLOOKUP(F31,'Source lists'!$E$1:F33,2,FALSE)</f>
+        <f>VLOOKUP(F31,'Source lists'!$E$1:F32,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J31" s="1">
-        <f>VLOOKUP(G31,'Source lists'!$H$1:I34,2,FALSE)</f>
+        <f>VLOOKUP(G31,'Source lists'!$H$1:I33,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K31" s="1">
         <f>VLOOKUP(F31,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G31,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H31,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
@@ -4852,11 +4901,11 @@
         <v>23</v>
       </c>
       <c r="I32" s="1">
-        <f>VLOOKUP(F32,'Source lists'!$E$1:F34,2,FALSE)</f>
+        <f>VLOOKUP(F32,'Source lists'!$E$1:F33,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J32" s="1">
-        <f>VLOOKUP(G32,'Source lists'!$H$1:I35,2,FALSE)</f>
+        <f>VLOOKUP(G32,'Source lists'!$H$1:I34,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K32" s="1">
@@ -4864,9 +4913,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>38</v>
@@ -4874,11 +4923,8 @@
       <c r="C33" t="s">
         <v>80</v>
       </c>
-      <c r="D33" t="s">
-        <v>85</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -4890,11 +4936,11 @@
         <v>23</v>
       </c>
       <c r="I33" s="1">
-        <f>VLOOKUP(F33,'Source lists'!$E$1:F35,2,FALSE)</f>
+        <f>VLOOKUP(F33,'Source lists'!$E$1:F34,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J33" s="1">
-        <f>VLOOKUP(G33,'Source lists'!$H$1:I36,2,FALSE)</f>
+        <f>VLOOKUP(G33,'Source lists'!$H$1:I35,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K33" s="1">
@@ -4902,18 +4948,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="D34" t="s">
+        <v>85</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
@@ -4925,11 +4974,11 @@
         <v>23</v>
       </c>
       <c r="I34" s="1">
-        <f>VLOOKUP(F34,'Source lists'!$E$1:F36,2,FALSE)</f>
+        <f>VLOOKUP(F34,'Source lists'!$E$1:F35,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J34" s="1">
-        <f>VLOOKUP(G34,'Source lists'!$H$1:I37,2,FALSE)</f>
+        <f>VLOOKUP(G34,'Source lists'!$H$1:I36,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K34" s="1">
@@ -4939,16 +4988,16 @@
     </row>
     <row r="35" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F35" t="s">
         <v>15</v>
@@ -4960,11 +5009,11 @@
         <v>23</v>
       </c>
       <c r="I35" s="1">
-        <f>VLOOKUP(F35,'Source lists'!$E$1:F37,2,FALSE)</f>
+        <f>VLOOKUP(F35,'Source lists'!$E$1:F36,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J35" s="1">
-        <f>VLOOKUP(G35,'Source lists'!$H$1:I38,2,FALSE)</f>
+        <f>VLOOKUP(G35,'Source lists'!$H$1:I37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K35" s="1">
@@ -4972,18 +5021,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -4995,11 +5044,11 @@
         <v>23</v>
       </c>
       <c r="I36" s="1">
-        <f>VLOOKUP(F36,'Source lists'!$E$1:F38,2,FALSE)</f>
+        <f>VLOOKUP(F36,'Source lists'!$E$1:F37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J36" s="1">
-        <f>VLOOKUP(G36,'Source lists'!$H$1:I39,2,FALSE)</f>
+        <f>VLOOKUP(G36,'Source lists'!$H$1:I38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K36" s="1">
@@ -5007,9 +5056,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
@@ -5018,7 +5067,7 @@
         <v>106</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -5030,11 +5079,11 @@
         <v>23</v>
       </c>
       <c r="I37" s="1">
-        <f>VLOOKUP(F37,'Source lists'!$E$1:F39,2,FALSE)</f>
+        <f>VLOOKUP(F37,'Source lists'!$E$1:F38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J37" s="1">
-        <f>VLOOKUP(G37,'Source lists'!$H$1:I40,2,FALSE)</f>
+        <f>VLOOKUP(G37,'Source lists'!$H$1:I39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K37" s="1">
@@ -5042,18 +5091,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
@@ -5065,11 +5114,11 @@
         <v>23</v>
       </c>
       <c r="I38" s="1">
-        <f>VLOOKUP(F38,'Source lists'!$E$1:F40,2,FALSE)</f>
+        <f>VLOOKUP(F38,'Source lists'!$E$1:F39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J38" s="1">
-        <f>VLOOKUP(G38,'Source lists'!$H$1:I41,2,FALSE)</f>
+        <f>VLOOKUP(G38,'Source lists'!$H$1:I40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K38" s="1">
@@ -5077,9 +5126,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -5088,7 +5137,7 @@
         <v>150</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F39" t="s">
         <v>15</v>
@@ -5100,11 +5149,11 @@
         <v>23</v>
       </c>
       <c r="I39" s="1">
-        <f>VLOOKUP(F39,'Source lists'!$E$1:F41,2,FALSE)</f>
+        <f>VLOOKUP(F39,'Source lists'!$E$1:F40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J39" s="1">
-        <f>VLOOKUP(G39,'Source lists'!$H$1:I42,2,FALSE)</f>
+        <f>VLOOKUP(G39,'Source lists'!$H$1:I41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K39" s="1">
@@ -5112,18 +5161,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
@@ -5135,11 +5184,11 @@
         <v>23</v>
       </c>
       <c r="I40" s="1">
-        <f>VLOOKUP(F40,'Source lists'!$E$1:F42,2,FALSE)</f>
+        <f>VLOOKUP(F40,'Source lists'!$E$1:F41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J40" s="1">
-        <f>VLOOKUP(G40,'Source lists'!$H$1:I43,2,FALSE)</f>
+        <f>VLOOKUP(G40,'Source lists'!$H$1:I42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K40" s="1">
@@ -5149,16 +5198,16 @@
     </row>
     <row r="41" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F41" t="s">
         <v>15</v>
@@ -5170,11 +5219,11 @@
         <v>23</v>
       </c>
       <c r="I41" s="1">
-        <f>VLOOKUP(F41,'Source lists'!$E$1:F43,2,FALSE)</f>
+        <f>VLOOKUP(F41,'Source lists'!$E$1:F42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J41" s="1">
-        <f>VLOOKUP(G41,'Source lists'!$H$1:I44,2,FALSE)</f>
+        <f>VLOOKUP(G41,'Source lists'!$H$1:I43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K41" s="1">
@@ -5182,21 +5231,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
@@ -5208,24 +5254,21 @@
         <v>23</v>
       </c>
       <c r="I42" s="1">
-        <f>VLOOKUP(F42,'Source lists'!$E$1:F44,2,FALSE)</f>
+        <f>VLOOKUP(F42,'Source lists'!$E$1:F43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J42" s="1">
-        <f>VLOOKUP(G42,'Source lists'!$H$1:I45,2,FALSE)</f>
+        <f>VLOOKUP(G42,'Source lists'!$H$1:I44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K42" s="1">
         <f>VLOOKUP(F42,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G42,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H42,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L42">
-        <v>8</v>
-      </c>
     </row>
     <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -5237,33 +5280,36 @@
         <v>44</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>46</v>
+        <v>180</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
       </c>
       <c r="G43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H43" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="I43" s="1">
-        <f>VLOOKUP(F43,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <f>VLOOKUP(F43,'Source lists'!$E$1:F44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J43" s="1">
-        <f>VLOOKUP(G43,'Source lists'!$H$1:I46,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(G43,'Source lists'!$H$1:I45,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K43" s="1">
         <f>VLOOKUP(F43,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G43,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H43,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="L43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -5271,69 +5317,72 @@
       <c r="C44" t="s">
         <v>42</v>
       </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
       <c r="E44" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G44" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H44" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="I44" s="1">
-        <f>VLOOKUP(F44,'Source lists'!$E$1:F46,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F44,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J44" s="1">
-        <f>VLOOKUP(G44,'Source lists'!$H$1:I47,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G44,'Source lists'!$H$1:I46,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K44" s="1">
         <f>VLOOKUP(F44,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G44,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H44,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="F45" t="s">
         <v>16</v>
       </c>
       <c r="G45" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="H45" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="I45" s="1">
-        <f>VLOOKUP(F45,'Source lists'!$E$1:F47,2,FALSE)</f>
+        <f>VLOOKUP(F45,'Source lists'!$E$1:F46,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J45" s="1">
-        <f>VLOOKUP(G45,'Source lists'!$H$1:I48,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G45,'Source lists'!$H$1:I47,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K45" s="1">
         <f>VLOOKUP(F45,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G45,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H45,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -5342,7 +5391,7 @@
         <v>87</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F46" t="s">
         <v>16</v>
@@ -5354,11 +5403,11 @@
         <v>67</v>
       </c>
       <c r="I46" s="1">
-        <f>VLOOKUP(F46,'Source lists'!$E$1:F48,2,FALSE)</f>
+        <f>VLOOKUP(F46,'Source lists'!$E$1:F47,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J46" s="1">
-        <f>VLOOKUP(G46,'Source lists'!$H$1:I49,2,FALSE)</f>
+        <f>VLOOKUP(G46,'Source lists'!$H$1:I48,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K46" s="1">
@@ -5366,53 +5415,53 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F47" t="s">
         <v>16</v>
       </c>
       <c r="G47" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="H47" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="I47" s="1">
-        <f>VLOOKUP(F47,'Source lists'!$E$1:F49,2,FALSE)</f>
+        <f>VLOOKUP(F47,'Source lists'!$E$1:F48,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J47" s="1">
-        <f>VLOOKUP(G47,'Source lists'!$H$1:I50,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G47,'Source lists'!$H$1:I49,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K47" s="1">
         <f>VLOOKUP(F47,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G47,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H47,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
@@ -5424,11 +5473,11 @@
         <v>25</v>
       </c>
       <c r="I48" s="1">
-        <f>VLOOKUP(F48,'Source lists'!$E$1:F50,2,FALSE)</f>
+        <f>VLOOKUP(F48,'Source lists'!$E$1:F49,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J48" s="1">
-        <f>VLOOKUP(G48,'Source lists'!$H$1:I51,2,FALSE)</f>
+        <f>VLOOKUP(G48,'Source lists'!$H$1:I50,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K48" s="1">
@@ -5437,93 +5486,90 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
+      <c r="A49">
+        <v>57</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="F49" s="3" t="s">
+      <c r="E49" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F49" t="s">
         <v>16</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="H49" t="s">
         <v>25</v>
       </c>
-      <c r="I49" s="5">
-        <f>VLOOKUP(F49,'Source lists'!$E$1:F51,2,FALSE)</f>
+      <c r="I49" s="1">
+        <f>VLOOKUP(F49,'Source lists'!$E$1:F50,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="J49" s="5">
-        <f>VLOOKUP(G49,'Source lists'!$H$1:I52,2,FALSE)</f>
+      <c r="J49" s="1">
+        <f>VLOOKUP(G49,'Source lists'!$H$1:I51,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="K49" s="5">
+      <c r="K49" s="1">
         <f>VLOOKUP(F49,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G49,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H49,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3" t="s">
+    </row>
+    <row r="50" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>106</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" s="5">
+        <f>VLOOKUP(F50,'Source lists'!$E$1:F51,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="J50" s="5">
+        <f>VLOOKUP(G50,'Source lists'!$H$1:I52,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="K50" s="5">
+        <f>VLOOKUP(F50,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G50,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H50,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G50" t="s">
-        <v>28</v>
-      </c>
-      <c r="H50" t="s">
-        <v>24</v>
-      </c>
-      <c r="I50" s="1">
-        <f>VLOOKUP(F50,'Source lists'!$E$1:F52,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="J50" s="1">
-        <f>VLOOKUP(G50,'Source lists'!$H$1:I53,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="K50" s="1">
-        <f>VLOOKUP(F50,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G50,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H50,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>21.333333333333332</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="F51" t="s">
         <v>15</v>
@@ -5535,11 +5581,11 @@
         <v>24</v>
       </c>
       <c r="I51" s="1">
-        <f>VLOOKUP(F51,'Source lists'!$E$1:F53,2,FALSE)</f>
+        <f>VLOOKUP(F51,'Source lists'!$E$1:F52,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J51" s="1">
-        <f>VLOOKUP(G51,'Source lists'!$H$1:I54,2,FALSE)</f>
+        <f>VLOOKUP(G51,'Source lists'!$H$1:I53,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K51" s="1">
@@ -5547,18 +5593,21 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="D52" t="s">
+        <v>188</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="F52" t="s">
         <v>15</v>
@@ -5570,11 +5619,11 @@
         <v>24</v>
       </c>
       <c r="I52" s="1">
-        <f>VLOOKUP(F52,'Source lists'!$E$1:F54,2,FALSE)</f>
+        <f>VLOOKUP(F52,'Source lists'!$E$1:F53,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J52" s="1">
-        <f>VLOOKUP(G52,'Source lists'!$H$1:I55,2,FALSE)</f>
+        <f>VLOOKUP(G52,'Source lists'!$H$1:I54,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K52" s="1">
@@ -5584,16 +5633,16 @@
     </row>
     <row r="53" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -5605,11 +5654,11 @@
         <v>24</v>
       </c>
       <c r="I53" s="1">
-        <f>VLOOKUP(F53,'Source lists'!$E$1:F55,2,FALSE)</f>
+        <f>VLOOKUP(F53,'Source lists'!$E$1:F54,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J53" s="1">
-        <f>VLOOKUP(G53,'Source lists'!$H$1:I56,2,FALSE)</f>
+        <f>VLOOKUP(G53,'Source lists'!$H$1:I55,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K53" s="1">
@@ -5619,16 +5668,16 @@
     </row>
     <row r="54" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
@@ -5640,11 +5689,11 @@
         <v>24</v>
       </c>
       <c r="I54" s="1">
-        <f>VLOOKUP(F54,'Source lists'!$E$1:F56,2,FALSE)</f>
+        <f>VLOOKUP(F54,'Source lists'!$E$1:F55,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J54" s="1">
-        <f>VLOOKUP(G54,'Source lists'!$H$1:I57,2,FALSE)</f>
+        <f>VLOOKUP(G54,'Source lists'!$H$1:I56,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K54" s="1">
@@ -5652,18 +5701,18 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
@@ -5675,11 +5724,11 @@
         <v>24</v>
       </c>
       <c r="I55" s="1">
-        <f>VLOOKUP(F55,'Source lists'!$E$1:F57,2,FALSE)</f>
+        <f>VLOOKUP(F55,'Source lists'!$E$1:F56,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J55" s="1">
-        <f>VLOOKUP(G55,'Source lists'!$H$1:I58,2,FALSE)</f>
+        <f>VLOOKUP(G55,'Source lists'!$H$1:I57,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K55" s="1">
@@ -5689,7 +5738,7 @@
     </row>
     <row r="56" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -5698,7 +5747,7 @@
         <v>154</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
@@ -5710,11 +5759,11 @@
         <v>24</v>
       </c>
       <c r="I56" s="1">
-        <f>VLOOKUP(F56,'Source lists'!$E$1:F58,2,FALSE)</f>
+        <f>VLOOKUP(F56,'Source lists'!$E$1:F57,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J56" s="1">
-        <f>VLOOKUP(G56,'Source lists'!$H$1:I59,2,FALSE)</f>
+        <f>VLOOKUP(G56,'Source lists'!$H$1:I58,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K56" s="1">
@@ -5722,47 +5771,44 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
       </c>
       <c r="G57" t="s">
-        <v>159</v>
+        <v>28</v>
       </c>
       <c r="H57" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="I57" s="1">
-        <f>VLOOKUP(F57,'Source lists'!$E$1:F59,2,FALSE)</f>
+        <f>VLOOKUP(F57,'Source lists'!$E$1:F58,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J57" s="1">
-        <f>VLOOKUP(G57,'Source lists'!$H$1:I60,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G57,'Source lists'!$H$1:I59,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K57" s="1">
         <f>VLOOKUP(F57,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G57,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H57,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>20.571428571428573</v>
+        <v>21.333333333333332</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -5774,7 +5820,7 @@
         <v>54</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -5786,11 +5832,11 @@
         <v>69</v>
       </c>
       <c r="I58" s="1">
-        <f>VLOOKUP(F58,'Source lists'!$E$1:F60,2,FALSE)</f>
+        <f>VLOOKUP(F58,'Source lists'!$E$1:F59,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J58" s="1">
-        <f>VLOOKUP(G58,'Source lists'!$H$1:I61,2,FALSE)</f>
+        <f>VLOOKUP(G58,'Source lists'!$H$1:I60,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K58" s="1">
@@ -5800,7 +5846,7 @@
     </row>
     <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -5812,7 +5858,7 @@
         <v>54</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F59" t="s">
         <v>15</v>
@@ -5824,11 +5870,11 @@
         <v>69</v>
       </c>
       <c r="I59" s="1">
-        <f>VLOOKUP(F59,'Source lists'!$E$1:F61,2,FALSE)</f>
+        <f>VLOOKUP(F59,'Source lists'!$E$1:F60,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J59" s="1">
-        <f>VLOOKUP(G59,'Source lists'!$H$1:I62,2,FALSE)</f>
+        <f>VLOOKUP(G59,'Source lists'!$H$1:I61,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K59" s="1">
@@ -5838,7 +5884,7 @@
     </row>
     <row r="60" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
@@ -5850,7 +5896,7 @@
         <v>54</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F60" t="s">
         <v>15</v>
@@ -5862,11 +5908,11 @@
         <v>69</v>
       </c>
       <c r="I60" s="1">
-        <f>VLOOKUP(F60,'Source lists'!$E$1:F62,2,FALSE)</f>
+        <f>VLOOKUP(F60,'Source lists'!$E$1:F61,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J60" s="1">
-        <f>VLOOKUP(G60,'Source lists'!$H$1:I63,2,FALSE)</f>
+        <f>VLOOKUP(G60,'Source lists'!$H$1:I62,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K60" s="1">
@@ -5876,7 +5922,7 @@
     </row>
     <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
@@ -5888,7 +5934,7 @@
         <v>54</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F61" t="s">
         <v>15</v>
@@ -5900,11 +5946,11 @@
         <v>69</v>
       </c>
       <c r="I61" s="1">
-        <f>VLOOKUP(F61,'Source lists'!$E$1:F63,2,FALSE)</f>
+        <f>VLOOKUP(F61,'Source lists'!$E$1:F62,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J61" s="1">
-        <f>VLOOKUP(G61,'Source lists'!$H$1:I64,2,FALSE)</f>
+        <f>VLOOKUP(G61,'Source lists'!$H$1:I63,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K61" s="1">
@@ -5912,53 +5958,56 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>106</v>
+        <v>42</v>
+      </c>
+      <c r="D62" t="s">
+        <v>54</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>190</v>
+        <v>60</v>
       </c>
       <c r="F62" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G62" t="s">
         <v>159</v>
       </c>
       <c r="H62" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="I62" s="1">
-        <f>VLOOKUP(F62,'Source lists'!$E$1:F64,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F62,'Source lists'!$E$1:F63,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J62" s="1">
-        <f>VLOOKUP(G62,'Source lists'!$H$1:I65,2,FALSE)</f>
+        <f>VLOOKUP(G62,'Source lists'!$H$1:I64,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K62" s="1">
         <f>VLOOKUP(F62,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G62,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H62,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>18</v>
+        <v>20.571428571428573</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>141</v>
+        <v>190</v>
       </c>
       <c r="F63" t="s">
         <v>17</v>
@@ -5970,11 +6019,11 @@
         <v>23</v>
       </c>
       <c r="I63" s="1">
-        <f>VLOOKUP(F63,'Source lists'!$E$1:F65,2,FALSE)</f>
+        <f>VLOOKUP(F63,'Source lists'!$E$1:F64,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J63" s="1">
-        <f>VLOOKUP(G63,'Source lists'!$H$1:I66,2,FALSE)</f>
+        <f>VLOOKUP(G63,'Source lists'!$H$1:I65,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K63" s="1">
@@ -5984,89 +6033,86 @@
     </row>
     <row r="64" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>133</v>
-      </c>
-      <c r="D64" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F64" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G64" t="s">
-        <v>28</v>
+        <v>159</v>
       </c>
       <c r="H64" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="I64" s="1">
-        <f>VLOOKUP(F64,'Source lists'!$E$1:F66,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F64,'Source lists'!$E$1:F65,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J64" s="1">
-        <f>VLOOKUP(G64,'Source lists'!$H$1:I67,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G64,'Source lists'!$H$1:I66,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K64" s="1">
         <f>VLOOKUP(F64,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G64,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H64,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>161</v>
+        <v>133</v>
+      </c>
+      <c r="D65" t="s">
+        <v>188</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="F65" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G65" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I65" s="1">
-        <f>VLOOKUP(F65,'Source lists'!$E$1:F67,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F65,'Source lists'!$E$1:F66,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J65" s="1">
-        <f>VLOOKUP(G65,'Source lists'!$H$1:I68,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(G65,'Source lists'!$H$1:I67,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K65" s="1">
         <f>VLOOKUP(F65,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G65,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H65,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="L65">
-        <v>59</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>167</v>
@@ -6081,11 +6127,11 @@
         <v>69</v>
       </c>
       <c r="I66" s="1">
-        <f>VLOOKUP(F66,'Source lists'!$E$1:F68,2,FALSE)</f>
+        <f>VLOOKUP(F66,'Source lists'!$E$1:F67,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J66" s="1">
-        <f>VLOOKUP(G66,'Source lists'!$H$1:I69,2,FALSE)</f>
+        <f>VLOOKUP(G66,'Source lists'!$H$1:I68,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K66" s="1">
@@ -6093,18 +6139,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L66">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>167</v>
@@ -6119,11 +6165,11 @@
         <v>69</v>
       </c>
       <c r="I67" s="1">
-        <f>VLOOKUP(F67,'Source lists'!$E$1:F69,2,FALSE)</f>
+        <f>VLOOKUP(F67,'Source lists'!$E$1:F68,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J67" s="1">
-        <f>VLOOKUP(G67,'Source lists'!$H$1:I70,2,FALSE)</f>
+        <f>VLOOKUP(G67,'Source lists'!$H$1:I69,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K67" s="1">
@@ -6131,18 +6177,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L67">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B68" t="s">
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>167</v>
@@ -6157,11 +6203,11 @@
         <v>69</v>
       </c>
       <c r="I68" s="1">
-        <f>VLOOKUP(F68,'Source lists'!$E$1:F70,2,FALSE)</f>
+        <f>VLOOKUP(F68,'Source lists'!$E$1:F69,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J68" s="1">
-        <f>VLOOKUP(G68,'Source lists'!$H$1:I71,2,FALSE)</f>
+        <f>VLOOKUP(G68,'Source lists'!$H$1:I70,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K68" s="1">
@@ -6169,18 +6215,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L68">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>167</v>
@@ -6195,11 +6241,11 @@
         <v>69</v>
       </c>
       <c r="I69" s="1">
-        <f>VLOOKUP(F69,'Source lists'!$E$1:F71,2,FALSE)</f>
+        <f>VLOOKUP(F69,'Source lists'!$E$1:F70,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J69" s="1">
-        <f>VLOOKUP(G69,'Source lists'!$H$1:I72,2,FALSE)</f>
+        <f>VLOOKUP(G69,'Source lists'!$H$1:I71,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K69" s="1">
@@ -6207,18 +6253,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L69">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>167</v>
@@ -6233,11 +6279,11 @@
         <v>69</v>
       </c>
       <c r="I70" s="1">
-        <f>VLOOKUP(F70,'Source lists'!$E$1:F72,2,FALSE)</f>
+        <f>VLOOKUP(F70,'Source lists'!$E$1:F71,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J70" s="1">
-        <f>VLOOKUP(G70,'Source lists'!$H$1:I73,2,FALSE)</f>
+        <f>VLOOKUP(G70,'Source lists'!$H$1:I72,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K70" s="1">
@@ -6245,21 +6291,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L70">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -6271,11 +6317,11 @@
         <v>69</v>
       </c>
       <c r="I71" s="1">
-        <f>VLOOKUP(F71,'Source lists'!$E$1:F73,2,FALSE)</f>
+        <f>VLOOKUP(F71,'Source lists'!$E$1:F72,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J71" s="1">
-        <f>VLOOKUP(G71,'Source lists'!$H$1:I74,2,FALSE)</f>
+        <f>VLOOKUP(G71,'Source lists'!$H$1:I73,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K71" s="1">
@@ -6283,12 +6329,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L71">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
@@ -6309,11 +6355,11 @@
         <v>69</v>
       </c>
       <c r="I72" s="1">
-        <f>VLOOKUP(F72,'Source lists'!$E$1:F74,2,FALSE)</f>
+        <f>VLOOKUP(F72,'Source lists'!$E$1:F73,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J72" s="1">
-        <f>VLOOKUP(G72,'Source lists'!$H$1:I75,2,FALSE)</f>
+        <f>VLOOKUP(G72,'Source lists'!$H$1:I74,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K72" s="1">
@@ -6321,21 +6367,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L72">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F73" t="s">
         <v>17</v>
@@ -6347,11 +6393,11 @@
         <v>69</v>
       </c>
       <c r="I73" s="1">
-        <f>VLOOKUP(F73,'Source lists'!$E$1:F75,2,FALSE)</f>
+        <f>VLOOKUP(F73,'Source lists'!$E$1:F74,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J73" s="1">
-        <f>VLOOKUP(G73,'Source lists'!$H$1:I76,2,FALSE)</f>
+        <f>VLOOKUP(G73,'Source lists'!$H$1:I75,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K73" s="1">
@@ -6359,12 +6405,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L73">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
@@ -6373,7 +6419,7 @@
         <v>169</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F74" t="s">
         <v>17</v>
@@ -6385,11 +6431,11 @@
         <v>69</v>
       </c>
       <c r="I74" s="1">
-        <f>VLOOKUP(F74,'Source lists'!$E$1:F76,2,FALSE)</f>
+        <f>VLOOKUP(F74,'Source lists'!$E$1:F75,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J74" s="1">
-        <f>VLOOKUP(G74,'Source lists'!$H$1:I77,2,FALSE)</f>
+        <f>VLOOKUP(G74,'Source lists'!$H$1:I76,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K74" s="1">
@@ -6397,21 +6443,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L74">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F75" t="s">
         <v>17</v>
@@ -6423,11 +6469,11 @@
         <v>69</v>
       </c>
       <c r="I75" s="1">
-        <f>VLOOKUP(F75,'Source lists'!$E$1:F77,2,FALSE)</f>
+        <f>VLOOKUP(F75,'Source lists'!$E$1:F76,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J75" s="1">
-        <f>VLOOKUP(G75,'Source lists'!$H$1:I78,2,FALSE)</f>
+        <f>VLOOKUP(G75,'Source lists'!$H$1:I77,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K75" s="1">
@@ -6435,12 +6481,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L75">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
@@ -6449,7 +6495,7 @@
         <v>170</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="F76" t="s">
         <v>17</v>
@@ -6461,11 +6507,11 @@
         <v>69</v>
       </c>
       <c r="I76" s="1">
-        <f>VLOOKUP(F76,'Source lists'!$E$1:F78,2,FALSE)</f>
+        <f>VLOOKUP(F76,'Source lists'!$E$1:F77,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J76" s="1">
-        <f>VLOOKUP(G76,'Source lists'!$H$1:I79,2,FALSE)</f>
+        <f>VLOOKUP(G76,'Source lists'!$H$1:I78,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K76" s="1">
@@ -6473,56 +6519,59 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L76">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>84</v>
+        <v>172</v>
       </c>
       <c r="F77" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G77" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H77" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="I77" s="1">
-        <f>VLOOKUP(F77,'Source lists'!$E$1:F79,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F77,'Source lists'!$E$1:F78,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J77" s="1">
-        <f>VLOOKUP(G77,'Source lists'!$H$1:I80,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G77,'Source lists'!$H$1:I79,2,FALSE)</f>
+        <v>10</v>
       </c>
       <c r="K77" s="1">
         <f>VLOOKUP(F77,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G77,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H77,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>13.5</v>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="L77">
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A78">
+        <v>35</v>
+      </c>
+      <c r="B78" t="s">
         <v>38</v>
       </c>
-      <c r="B78" t="s">
-        <v>1</v>
-      </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
@@ -6534,11 +6583,11 @@
         <v>23</v>
       </c>
       <c r="I78" s="1">
-        <f>VLOOKUP(F78,'Source lists'!$E$1:F80,2,FALSE)</f>
+        <f>VLOOKUP(F78,'Source lists'!$E$1:F79,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J78" s="1">
-        <f>VLOOKUP(G78,'Source lists'!$H$1:I81,2,FALSE)</f>
+        <f>VLOOKUP(G78,'Source lists'!$H$1:I80,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K78" s="1">
@@ -6548,19 +6597,16 @@
     </row>
     <row r="79" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B79" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>133</v>
-      </c>
-      <c r="D79" t="s">
-        <v>188</v>
+        <v>87</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="F79" t="s">
         <v>16</v>
@@ -6572,11 +6618,11 @@
         <v>23</v>
       </c>
       <c r="I79" s="1">
-        <f>VLOOKUP(F79,'Source lists'!$E$1:F81,2,FALSE)</f>
+        <f>VLOOKUP(F79,'Source lists'!$E$1:F80,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J79" s="1">
-        <f>VLOOKUP(G79,'Source lists'!$H$1:I82,2,FALSE)</f>
+        <f>VLOOKUP(G79,'Source lists'!$H$1:I81,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K79" s="1">
@@ -6586,7 +6632,7 @@
     </row>
     <row r="80" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -6598,7 +6644,7 @@
         <v>188</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="F80" t="s">
         <v>16</v>
@@ -6610,11 +6656,11 @@
         <v>23</v>
       </c>
       <c r="I80" s="1">
-        <f>VLOOKUP(F80,'Source lists'!$E$1:F82,2,FALSE)</f>
+        <f>VLOOKUP(F80,'Source lists'!$E$1:F81,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J80" s="1">
-        <f>VLOOKUP(G80,'Source lists'!$H$1:I83,2,FALSE)</f>
+        <f>VLOOKUP(G80,'Source lists'!$H$1:I82,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K80" s="1">
@@ -6622,18 +6668,21 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>150</v>
+        <v>133</v>
+      </c>
+      <c r="D81" t="s">
+        <v>188</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="F81" t="s">
         <v>16</v>
@@ -6645,11 +6694,11 @@
         <v>23</v>
       </c>
       <c r="I81" s="1">
-        <f>VLOOKUP(F81,'Source lists'!$E$1:F83,2,FALSE)</f>
+        <f>VLOOKUP(F81,'Source lists'!$E$1:F82,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J81" s="1">
-        <f>VLOOKUP(G81,'Source lists'!$H$1:I84,2,FALSE)</f>
+        <f>VLOOKUP(G81,'Source lists'!$H$1:I83,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K81" s="1">
@@ -6659,7 +6708,7 @@
     </row>
     <row r="82" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
@@ -6668,7 +6717,7 @@
         <v>150</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F82" t="s">
         <v>16</v>
@@ -6680,11 +6729,11 @@
         <v>23</v>
       </c>
       <c r="I82" s="1">
-        <f>VLOOKUP(F82,'Source lists'!$E$1:F84,2,FALSE)</f>
+        <f>VLOOKUP(F82,'Source lists'!$E$1:F83,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J82" s="1">
-        <f>VLOOKUP(G82,'Source lists'!$H$1:I85,2,FALSE)</f>
+        <f>VLOOKUP(G82,'Source lists'!$H$1:I84,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K82" s="1">
@@ -6694,51 +6743,48 @@
     </row>
     <row r="83" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>73</v>
-      </c>
-      <c r="D83" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="F83" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G83" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H83" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="I83" s="1">
-        <f>VLOOKUP(F83,'Source lists'!$E$1:F85,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F83,'Source lists'!$E$1:F84,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J83" s="1">
-        <f>VLOOKUP(G83,'Source lists'!$H$1:I86,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G83,'Source lists'!$H$1:I85,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K83" s="1">
         <f>VLOOKUP(F83,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G83,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H83,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.8</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B84" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C84" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D84" t="s">
         <v>85</v>
@@ -6756,11 +6802,11 @@
         <v>70</v>
       </c>
       <c r="I84" s="1">
-        <f>VLOOKUP(F84,'Source lists'!$E$1:F86,2,FALSE)</f>
+        <f>VLOOKUP(F84,'Source lists'!$E$1:F85,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J84" s="1">
-        <f>VLOOKUP(G84,'Source lists'!$H$1:I87,2,FALSE)</f>
+        <f>VLOOKUP(G84,'Source lists'!$H$1:I86,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K84" s="1">
@@ -6768,21 +6814,21 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B85" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C85" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D85" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="F85" t="s">
         <v>15</v>
@@ -6794,11 +6840,11 @@
         <v>70</v>
       </c>
       <c r="I85" s="1">
-        <f>VLOOKUP(F85,'Source lists'!$E$1:F87,2,FALSE)</f>
+        <f>VLOOKUP(F85,'Source lists'!$E$1:F86,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J85" s="1">
-        <f>VLOOKUP(G85,'Source lists'!$H$1:I88,2,FALSE)</f>
+        <f>VLOOKUP(G85,'Source lists'!$H$1:I87,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K85" s="1">
@@ -6808,7 +6854,7 @@
     </row>
     <row r="86" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
@@ -6820,7 +6866,7 @@
         <v>112</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F86" t="s">
         <v>15</v>
@@ -6832,11 +6878,11 @@
         <v>70</v>
       </c>
       <c r="I86" s="1">
-        <f>VLOOKUP(F86,'Source lists'!$E$1:F88,2,FALSE)</f>
+        <f>VLOOKUP(F86,'Source lists'!$E$1:F87,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J86" s="1">
-        <f>VLOOKUP(G86,'Source lists'!$H$1:I89,2,FALSE)</f>
+        <f>VLOOKUP(G86,'Source lists'!$H$1:I88,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K86" s="1">
@@ -6846,7 +6892,7 @@
     </row>
     <row r="87" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
@@ -6854,8 +6900,11 @@
       <c r="C87" t="s">
         <v>91</v>
       </c>
+      <c r="D87" t="s">
+        <v>112</v>
+      </c>
       <c r="E87" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F87" t="s">
         <v>15</v>
@@ -6867,11 +6916,11 @@
         <v>70</v>
       </c>
       <c r="I87" s="1">
-        <f>VLOOKUP(F87,'Source lists'!$E$1:F89,2,FALSE)</f>
+        <f>VLOOKUP(F87,'Source lists'!$E$1:F88,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J87" s="1">
-        <f>VLOOKUP(G87,'Source lists'!$H$1:I90,2,FALSE)</f>
+        <f>VLOOKUP(G87,'Source lists'!$H$1:I89,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K87" s="1">
@@ -6879,56 +6928,56 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>87</v>
-      </c>
-      <c r="D88" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F88" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G88" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H88" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="I88" s="1">
-        <f>VLOOKUP(F88,'Source lists'!$E$1:F90,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F88,'Source lists'!$E$1:F89,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J88" s="1">
-        <f>VLOOKUP(G88,'Source lists'!$H$1:I91,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(G88,'Source lists'!$H$1:I90,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K88" s="1">
         <f>VLOOKUP(F88,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G88,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H88,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B89" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>104</v>
+        <v>87</v>
+      </c>
+      <c r="D89" t="s">
+        <v>89</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="F89" t="s">
         <v>17</v>
@@ -6940,11 +6989,11 @@
         <v>22</v>
       </c>
       <c r="I89" s="1">
-        <f>VLOOKUP(F89,'Source lists'!$E$1:F91,2,FALSE)</f>
+        <f>VLOOKUP(F89,'Source lists'!$E$1:F90,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J89" s="1">
-        <f>VLOOKUP(G89,'Source lists'!$H$1:I92,2,FALSE)</f>
+        <f>VLOOKUP(G89,'Source lists'!$H$1:I91,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K89" s="1">
@@ -6952,18 +7001,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B90" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="F90" t="s">
         <v>17</v>
@@ -6975,11 +7024,11 @@
         <v>22</v>
       </c>
       <c r="I90" s="1">
-        <f>VLOOKUP(F90,'Source lists'!$E$1:F92,2,FALSE)</f>
+        <f>VLOOKUP(F90,'Source lists'!$E$1:F91,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J90" s="1">
-        <f>VLOOKUP(G90,'Source lists'!$H$1:I93,2,FALSE)</f>
+        <f>VLOOKUP(G90,'Source lists'!$H$1:I92,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K90" s="1">
@@ -6987,18 +7036,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C91" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="F91" t="s">
         <v>17</v>
@@ -7010,11 +7059,11 @@
         <v>22</v>
       </c>
       <c r="I91" s="1">
-        <f>VLOOKUP(F91,'Source lists'!$E$1:F93,2,FALSE)</f>
+        <f>VLOOKUP(F91,'Source lists'!$E$1:F92,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J91" s="1">
-        <f>VLOOKUP(G91,'Source lists'!$H$1:I94,2,FALSE)</f>
+        <f>VLOOKUP(G91,'Source lists'!$H$1:I93,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K91" s="1">
@@ -7022,18 +7071,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="F92" t="s">
         <v>17</v>
@@ -7045,11 +7094,11 @@
         <v>22</v>
       </c>
       <c r="I92" s="1">
-        <f>VLOOKUP(F92,'Source lists'!$E$1:F94,2,FALSE)</f>
+        <f>VLOOKUP(F92,'Source lists'!$E$1:F93,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J92" s="1">
-        <f>VLOOKUP(G92,'Source lists'!$H$1:I95,2,FALSE)</f>
+        <f>VLOOKUP(G92,'Source lists'!$H$1:I94,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K92" s="1">
@@ -7057,18 +7106,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="F93" t="s">
         <v>17</v>
@@ -7080,11 +7129,11 @@
         <v>22</v>
       </c>
       <c r="I93" s="1">
-        <f>VLOOKUP(F93,'Source lists'!$E$1:F95,2,FALSE)</f>
+        <f>VLOOKUP(F93,'Source lists'!$E$1:F94,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J93" s="1">
-        <f>VLOOKUP(G93,'Source lists'!$H$1:I96,2,FALSE)</f>
+        <f>VLOOKUP(G93,'Source lists'!$H$1:I95,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K93" s="1">
@@ -7094,16 +7143,16 @@
     </row>
     <row r="94" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="B94" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>117</v>
+        <v>196</v>
       </c>
       <c r="F94" t="s">
         <v>17</v>
@@ -7112,30 +7161,33 @@
         <v>26</v>
       </c>
       <c r="H94" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I94" s="1">
-        <f>VLOOKUP(F94,'Source lists'!$E$1:F96,2,FALSE)</f>
+        <f>VLOOKUP(F94,'Source lists'!$E$1:F95,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J94" s="1">
-        <f>VLOOKUP(G94,'Source lists'!$H$1:I97,2,FALSE)</f>
+        <f>VLOOKUP(G94,'Source lists'!$H$1:I96,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K94" s="1">
         <f>VLOOKUP(F94,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G94,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H94,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B95" t="s">
-        <v>7</v>
+        <v>66</v>
+      </c>
+      <c r="C95" t="s">
+        <v>82</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F95" t="s">
         <v>17</v>
@@ -7147,11 +7199,11 @@
         <v>21</v>
       </c>
       <c r="I95" s="1">
-        <f>VLOOKUP(F95,'Source lists'!$E$1:F97,2,FALSE)</f>
+        <f>VLOOKUP(F95,'Source lists'!$E$1:F96,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J95" s="1">
-        <f>VLOOKUP(G95,'Source lists'!$H$1:I98,2,FALSE)</f>
+        <f>VLOOKUP(G95,'Source lists'!$H$1:I97,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K95" s="1">
@@ -7161,13 +7213,13 @@
     </row>
     <row r="96" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B96" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F96" t="s">
         <v>17</v>
@@ -7179,11 +7231,11 @@
         <v>21</v>
       </c>
       <c r="I96" s="1">
-        <f>VLOOKUP(F96,'Source lists'!$E$1:F98,2,FALSE)</f>
+        <f>VLOOKUP(F96,'Source lists'!$E$1:F97,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J96" s="1">
-        <f>VLOOKUP(G96,'Source lists'!$H$1:I99,2,FALSE)</f>
+        <f>VLOOKUP(G96,'Source lists'!$H$1:I98,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K96" s="1">
@@ -7191,18 +7243,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="F97" t="s">
         <v>17</v>
@@ -7214,11 +7263,11 @@
         <v>21</v>
       </c>
       <c r="I97" s="1">
-        <f>VLOOKUP(F97,'Source lists'!$E$1:F99,2,FALSE)</f>
+        <f>VLOOKUP(F97,'Source lists'!$E$1:F98,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J97" s="1">
-        <f>VLOOKUP(G97,'Source lists'!$H$1:I100,2,FALSE)</f>
+        <f>VLOOKUP(G97,'Source lists'!$H$1:I99,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K97" s="1">
@@ -7226,18 +7275,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B98" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F98" t="s">
         <v>17</v>
@@ -7249,11 +7298,11 @@
         <v>21</v>
       </c>
       <c r="I98" s="1">
-        <f>VLOOKUP(F98,'Source lists'!$E$1:F100,2,FALSE)</f>
+        <f>VLOOKUP(F98,'Source lists'!$E$1:F99,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J98" s="1">
-        <f>VLOOKUP(G98,'Source lists'!$H$1:I101,2,FALSE)</f>
+        <f>VLOOKUP(G98,'Source lists'!$H$1:I100,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K98" s="1">
@@ -7261,53 +7310,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>168</v>
+      </c>
+      <c r="C99" t="s">
+        <v>169</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F99" t="s">
+        <v>17</v>
+      </c>
+      <c r="G99" t="s">
         <v>26</v>
       </c>
-      <c r="B99" t="s">
-        <v>66</v>
-      </c>
-      <c r="C99" t="s">
-        <v>73</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F99" t="s">
-        <v>16</v>
-      </c>
-      <c r="G99" t="s">
-        <v>29</v>
-      </c>
       <c r="H99" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I99" s="1">
-        <f>VLOOKUP(F99,'Source lists'!$E$1:F101,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F99,'Source lists'!$E$1:F100,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J99" s="1">
-        <f>VLOOKUP(G99,'Source lists'!$H$1:I102,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G99,'Source lists'!$H$1:I101,2,FALSE)</f>
+        <v>10</v>
       </c>
       <c r="K99" s="1">
         <f>VLOOKUP(F99,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G99,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H99,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B100" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C100" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="F100" t="s">
         <v>16</v>
@@ -7319,11 +7368,11 @@
         <v>24</v>
       </c>
       <c r="I100" s="1">
-        <f>VLOOKUP(F100,'Source lists'!$E$1:F102,2,FALSE)</f>
+        <f>VLOOKUP(F100,'Source lists'!$E$1:F101,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J100" s="1">
-        <f>VLOOKUP(G100,'Source lists'!$H$1:I103,2,FALSE)</f>
+        <f>VLOOKUP(G100,'Source lists'!$H$1:I102,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K100" s="1">
@@ -7331,18 +7380,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="F101" t="s">
         <v>16</v>
@@ -7354,11 +7403,11 @@
         <v>24</v>
       </c>
       <c r="I101" s="1">
-        <f>VLOOKUP(F101,'Source lists'!$E$1:F103,2,FALSE)</f>
+        <f>VLOOKUP(F101,'Source lists'!$E$1:F102,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J101" s="1">
-        <f>VLOOKUP(G101,'Source lists'!$H$1:I104,2,FALSE)</f>
+        <f>VLOOKUP(G101,'Source lists'!$H$1:I103,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K101" s="1">
@@ -7366,9 +7415,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B102" t="s">
         <v>1</v>
@@ -7377,7 +7426,7 @@
         <v>91</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F102" t="s">
         <v>16</v>
@@ -7389,11 +7438,11 @@
         <v>24</v>
       </c>
       <c r="I102" s="1">
-        <f>VLOOKUP(F102,'Source lists'!$E$1:F104,2,FALSE)</f>
+        <f>VLOOKUP(F102,'Source lists'!$E$1:F103,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J102" s="1">
-        <f>VLOOKUP(G102,'Source lists'!$H$1:I105,2,FALSE)</f>
+        <f>VLOOKUP(G102,'Source lists'!$H$1:I104,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K102" s="1">
@@ -7401,44 +7450,44 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B103" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>199</v>
+        <v>98</v>
       </c>
       <c r="F103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G103" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="H103" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="I103" s="1">
-        <f>VLOOKUP(F103,'Source lists'!$E$1:F105,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F103,'Source lists'!$E$1:F104,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J103" s="1">
-        <f>VLOOKUP(G103,'Source lists'!$H$1:I106,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G103,'Source lists'!$H$1:I105,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K103" s="1">
         <f>VLOOKUP(F103,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G103,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H103,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B104" t="s">
         <v>2</v>
@@ -7447,7 +7496,7 @@
         <v>131</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F104" t="s">
         <v>17</v>
@@ -7459,11 +7508,11 @@
         <v>67</v>
       </c>
       <c r="I104" s="1">
-        <f>VLOOKUP(F104,'Source lists'!$E$1:F106,2,FALSE)</f>
+        <f>VLOOKUP(F104,'Source lists'!$E$1:F105,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J104" s="1">
-        <f>VLOOKUP(G104,'Source lists'!$H$1:I107,2,FALSE)</f>
+        <f>VLOOKUP(G104,'Source lists'!$H$1:I106,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K104" s="1">
@@ -7471,9 +7520,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B105" t="s">
         <v>2</v>
@@ -7482,7 +7531,7 @@
         <v>131</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="F105" t="s">
         <v>17</v>
@@ -7494,11 +7543,11 @@
         <v>67</v>
       </c>
       <c r="I105" s="1">
-        <f>VLOOKUP(F105,'Source lists'!$E$1:F107,2,FALSE)</f>
+        <f>VLOOKUP(F105,'Source lists'!$E$1:F106,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J105" s="1">
-        <f>VLOOKUP(G105,'Source lists'!$H$1:I108,2,FALSE)</f>
+        <f>VLOOKUP(G105,'Source lists'!$H$1:I107,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K105" s="1">
@@ -7506,21 +7555,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B106" t="s">
         <v>2</v>
       </c>
       <c r="C106" t="s">
-        <v>133</v>
-      </c>
-      <c r="D106" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>201</v>
+        <v>132</v>
       </c>
       <c r="F106" t="s">
         <v>17</v>
@@ -7532,11 +7578,11 @@
         <v>67</v>
       </c>
       <c r="I106" s="1">
-        <f>VLOOKUP(F106,'Source lists'!$E$1:F108,2,FALSE)</f>
+        <f>VLOOKUP(F106,'Source lists'!$E$1:F107,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J106" s="1">
-        <f>VLOOKUP(G106,'Source lists'!$H$1:I109,2,FALSE)</f>
+        <f>VLOOKUP(G106,'Source lists'!$H$1:I108,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K106" s="1">
@@ -7544,18 +7590,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="D107" t="s">
+        <v>138</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="F107" t="s">
         <v>17</v>
@@ -7567,11 +7616,11 @@
         <v>67</v>
       </c>
       <c r="I107" s="1">
-        <f>VLOOKUP(F107,'Source lists'!$E$1:F109,2,FALSE)</f>
+        <f>VLOOKUP(F107,'Source lists'!$E$1:F108,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J107" s="1">
-        <f>VLOOKUP(G107,'Source lists'!$H$1:I110,2,FALSE)</f>
+        <f>VLOOKUP(G107,'Source lists'!$H$1:I109,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K107" s="1">
@@ -7579,158 +7628,158 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="B108" t="s">
-        <v>75</v>
+        <v>3</v>
+      </c>
+      <c r="C108" t="s">
+        <v>142</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="F108" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G108" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="H108" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="I108" s="1">
-        <f>VLOOKUP(F108,'Source lists'!$E$1:F45,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F108,'Source lists'!$E$1:F109,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J108" s="1">
-        <f>VLOOKUP(G108,'Source lists'!$H$1:I46,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G108,'Source lists'!$H$1:I110,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K108" s="1">
         <f>VLOOKUP(F108,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G108,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H108,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="B109" t="s">
         <v>75</v>
       </c>
-      <c r="C109" t="s">
-        <v>102</v>
-      </c>
       <c r="E109" s="2" t="s">
-        <v>103</v>
+        <v>185</v>
       </c>
       <c r="F109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G109" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H109" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="I109" s="1">
-        <f>VLOOKUP(F109,'Source lists'!$E$1:F110,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F109,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J109" s="1">
-        <f>VLOOKUP(G109,'Source lists'!$H$1:I111,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(G109,'Source lists'!$H$1:I46,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K109" s="1">
         <f>VLOOKUP(F109,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G109,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H109,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>51</v>
+      </c>
+      <c r="B110" t="s">
+        <v>75</v>
+      </c>
+      <c r="C110" t="s">
+        <v>102</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F110" t="s">
+        <v>17</v>
+      </c>
+      <c r="G110" t="s">
+        <v>27</v>
+      </c>
+      <c r="H110" t="s">
+        <v>69</v>
+      </c>
+      <c r="I110" s="1">
+        <f>VLOOKUP(F110,'Source lists'!$E$1:F110,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J110" s="1">
+        <f>VLOOKUP(G110,'Source lists'!$H$1:I111,2,FALSE)</f>
         <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>28</v>
-      </c>
-      <c r="B110" t="s">
-        <v>66</v>
-      </c>
-      <c r="C110" t="s">
-        <v>73</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F110" t="s">
-        <v>16</v>
-      </c>
-      <c r="G110" t="s">
-        <v>29</v>
-      </c>
-      <c r="H110" t="s">
-        <v>67</v>
-      </c>
-      <c r="I110" s="1">
-        <f>VLOOKUP(F110,'Source lists'!$E$1:F111,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="J110" s="1">
-        <f>VLOOKUP(G110,'Source lists'!$H$1:I112,2,FALSE)</f>
-        <v>3</v>
       </c>
       <c r="K110" s="1">
         <f>VLOOKUP(F110,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G110,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H110,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="B111" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C111" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="F111" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G111" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H111" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="I111" s="1">
-        <f>VLOOKUP(F111,'Source lists'!$E$1:F46,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F111,'Source lists'!$E$1:F111,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J111" s="1">
-        <f>VLOOKUP(G111,'Source lists'!$H$1:I47,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(G111,'Source lists'!$H$1:I112,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K111" s="1">
         <f>VLOOKUP(F111,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G111,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H111,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A112">
-        <v>29</v>
-      </c>
-      <c r="B112" t="s">
-        <v>66</v>
-      </c>
       <c r="C112" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="F112" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G112" t="s">
         <v>30</v>
@@ -7739,27 +7788,27 @@
         <v>23</v>
       </c>
       <c r="I112" s="1">
-        <f>VLOOKUP(F112,'Source lists'!$E$1:F112,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F112,'Source lists'!$E$1:F46,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J112" s="1">
-        <f>VLOOKUP(G112,'Source lists'!$H$1:I113,2,FALSE)</f>
+        <f>VLOOKUP(G112,'Source lists'!$H$1:I47,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K112" s="1">
         <f>VLOOKUP(F112,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G112,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H112,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>1.5</v>
-      </c>
-      <c r="L112">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B113" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="C113" t="s">
+        <v>73</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>79</v>
@@ -7774,11 +7823,11 @@
         <v>23</v>
       </c>
       <c r="I113" s="1">
-        <f>VLOOKUP(F113,'Source lists'!$E$1:F113,2,FALSE)</f>
+        <f>VLOOKUP(F113,'Source lists'!$E$1:F112,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J113" s="1">
-        <f>VLOOKUP(G113,'Source lists'!$H$1:I114,2,FALSE)</f>
+        <f>VLOOKUP(G113,'Source lists'!$H$1:I113,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K113" s="1">
@@ -7791,16 +7840,13 @@
     </row>
     <row r="114" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B114" t="s">
-        <v>75</v>
-      </c>
-      <c r="C114" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F114" t="s">
         <v>16</v>
@@ -7809,25 +7855,63 @@
         <v>30</v>
       </c>
       <c r="H114" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="I114" s="1">
-        <f>VLOOKUP(F114,'Source lists'!$E$1:F114,2,FALSE)</f>
+        <f>VLOOKUP(F114,'Source lists'!$E$1:F113,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J114" s="1">
-        <f>VLOOKUP(G114,'Source lists'!$H$1:I115,2,FALSE)</f>
+        <f>VLOOKUP(G114,'Source lists'!$H$1:I114,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K114" s="1">
         <f>VLOOKUP(F114,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G114,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H114,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="L114">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>27</v>
+      </c>
+      <c r="B115" t="s">
+        <v>75</v>
+      </c>
+      <c r="C115" t="s">
+        <v>76</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F115" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" t="s">
+        <v>30</v>
+      </c>
+      <c r="H115" t="s">
+        <v>69</v>
+      </c>
+      <c r="I115" s="1">
+        <f>VLOOKUP(F115,'Source lists'!$E$1:F114,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="J115" s="1">
+        <f>VLOOKUP(G115,'Source lists'!$H$1:I115,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K115" s="1">
+        <f>VLOOKUP(F115,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G115,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H115,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>0.42857142857142855</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M114">
-      <sortCondition descending="1" ref="K1:K114"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M115">
+      <sortCondition descending="1" ref="K1:K115"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sigmafox/modals/register: Now built for use
</commit_message>
<xml_diff>
--- a/e-Question - To do list.xlsx
+++ b/e-Question - To do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25BFD44-393C-FA46-A2C1-66E223562EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D20CC61-7CD2-F343-9777-5A6CD0027F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of completion" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="18" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="211">
   <si>
     <t>Sections</t>
   </si>
@@ -707,10 +707,10 @@
     <t>Register modal</t>
   </si>
   <si>
-    <t>Needs to be a modal specfically for modals</t>
-  </si>
-  <si>
     <t xml:space="preserve">Payment are not being recorded correctly </t>
+  </si>
+  <si>
+    <t>Needs to be a modal specfically for registrations</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45307.534193402775" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="116" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45307.544524074074" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="115" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:M1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
@@ -857,7 +857,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="116">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="115">
   <r>
     <n v="53"/>
     <s v="Calendar/Appointments"/>
@@ -946,7 +946,7 @@
     <n v="6"/>
     <n v="96"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="45"/>
@@ -2583,82 +2583,11 @@
     <m/>
     <x v="1"/>
   </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colFields count="1">
-    <field x="12"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Priority S" fld="10" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:D15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2713,8 +2642,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2756,6 +2685,62 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Importance S" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="12"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Priority S" fld="10" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3068,25 +3053,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CCC35A-14FA-1E40-8319-0349AC17C33D}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
-      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" max="3" activeRow="1" activeCol="1" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="12" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3110,19 +3085,19 @@
         <v>206</v>
       </c>
       <c r="B3" s="8">
-        <v>845</v>
+        <v>941</v>
       </c>
       <c r="C3" s="8">
-        <v>2278.5976190476185</v>
+        <v>2182.5976190476181</v>
       </c>
       <c r="D3" s="8">
-        <v>3123.5976190476185</v>
+        <v>3123.5976190476181</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="7">
         <f>GETPIVOTDATA("Priority S",$A$1,"Status","Done")/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.27052139969860767</v>
+        <v>0.3012551918537158</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3146,10 +3121,10 @@
         <v>183</v>
       </c>
       <c r="B9" s="8">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C9" s="8">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D9" s="8">
         <v>364</v>
@@ -3158,7 +3133,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="7">
         <f>GETPIVOTDATA("Importance S",$A$7,"Status","Done")/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.17857142857142858</v>
+        <v>0.20054945054945056</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3182,10 +3157,10 @@
         <v>184</v>
       </c>
       <c r="B15" s="8">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C15" s="8">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="D15" s="8">
         <v>663</v>
@@ -3194,7 +3169,7 @@
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="7">
         <f>GETPIVOTDATA("Impact S",$A$13,"Status","Done")/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>8.4464555052790352E-2</v>
+        <v>9.3514328808446456E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3625,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3894,43 +3869,45 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>114</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D7"/>
-      <c r="E7" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="5">
         <f>VLOOKUP(F7,'Source lists'!$E$1:F119,2,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="5">
         <f>VLOOKUP(G7,'Source lists'!$H$1:I120,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="5">
         <f>VLOOKUP(F7,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G7,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H7,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>96</v>
       </c>
-      <c r="L7"/>
-      <c r="M7"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -4025,7 +4002,7 @@
         <v>208</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>

</xml_diff>